<commit_message>
Update xlsx template per suggestions by @hackstock
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE132C7-61B1-7C44-94F9-CCEF0BEB22D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B282BD-5D0B-1742-A54F-53F0F96663C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21820" windowHeight="14620" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
-    <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="Regions" sheetId="3" r:id="rId3"/>
+    <sheet name="Regions" sheetId="3" r:id="rId2"/>
+    <sheet name="Users" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -52,46 +52,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>User1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Model (including version number)</t>
   </si>
   <si>
@@ -159,6 +119,9 @@
   </si>
   <si>
     <t>Check the project GitHub repository for region names and definitions</t>
+  </si>
+  <si>
+    <t>All users listed here will have "EDIT" permission for the model version(s) listed in the "Model" sheet</t>
   </si>
 </sst>
 </file>
@@ -660,24 +623,24 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -690,150 +653,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F604CE36-32F7-4568-80C0-72A2E5C96CDB}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{3EB41CE9-2C1F-8145-828E-109A4D64B189}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{7C30ABF4-DB22-BD45-9F7B-B75FCD6038DE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643947D9-83D7-476A-BAA5-689C7FE1BE65}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -854,62 +679,62 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="10" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="F3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="10" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1028,4 +853,128 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F604CE36-32F7-4568-80C0-72A2E5C96CDB}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{3EB41CE9-2C1F-8145-828E-109A4D64B189}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{7C30ABF4-DB22-BD45-9F7B-B75FCD6038DE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add name-override from pycountry package
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52C331-6745-1945-B300-D1256730E721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E6F85-75BB-DA4A-8CD4-54615B5DED4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="949">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -839,42 +839,18 @@
     <t>Bonaire, Sint Eustatius and Saba</t>
   </si>
   <si>
-    <t>Bolivia, Plurinational State of</t>
-  </si>
-  <si>
     <t>Congo, The Democratic Republic of the</t>
   </si>
   <si>
-    <t>Micronesia, Federated States of</t>
-  </si>
-  <si>
-    <t>Iran, Islamic Republic of</t>
-  </si>
-  <si>
     <t>Korea, Republic of</t>
   </si>
   <si>
-    <t>Moldova, Republic of</t>
-  </si>
-  <si>
-    <t>Korea, Democratic People's Republic of</t>
-  </si>
-  <si>
-    <t>Palestine, State of</t>
-  </si>
-  <si>
     <t>Saint Helena, Ascension and Tristan da Cunha</t>
   </si>
   <si>
     <t>Taiwan, Province of China</t>
   </si>
   <si>
-    <t>Tanzania, United Republic of</t>
-  </si>
-  <si>
-    <t>Venezuela, Bolivarian Republic of</t>
-  </si>
-  <si>
     <t>Virgin Islands, British</t>
   </si>
   <si>
@@ -2871,6 +2847,48 @@
   </si>
   <si>
     <t>Republic of Zimbabwe</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Vatican</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>The Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
   </si>
 </sst>
 </file>
@@ -3650,7 +3668,7 @@
         <v>261</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>262</v>
@@ -3667,13 +3685,13 @@
         <v>90</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>11</v>
@@ -3686,10 +3704,10 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E5" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3698,13 +3716,13 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E6" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3713,13 +3731,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="D7" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="E7" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3728,10 +3746,10 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E8" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3740,10 +3758,10 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E9" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3752,13 +3770,13 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="D10" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E10" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3767,13 +3785,13 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="D11" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="E11" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3782,10 +3800,10 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E12" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3794,13 +3812,13 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="D13" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E13" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,13 +3827,13 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D14" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E14" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3824,10 +3842,10 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E15" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3836,10 +3854,10 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E16" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3848,10 +3866,10 @@
         <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E17" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3860,10 +3878,10 @@
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E18" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3872,10 +3890,10 @@
         <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E19" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3884,13 +3902,13 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="D20" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E20" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3899,13 +3917,13 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="D21" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E21" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3914,13 +3932,13 @@
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="D22" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="E22" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3929,13 +3947,13 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="D23" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E23" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3944,13 +3962,13 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="D24" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E24" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3962,10 +3980,10 @@
         <v>264</v>
       </c>
       <c r="D25" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E25" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3974,10 +3992,10 @@
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E26" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3986,13 +4004,13 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="D27" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E27" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4001,13 +4019,13 @@
         <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="D28" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E28" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4016,13 +4034,13 @@
         <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E29" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -4031,13 +4049,13 @@
         <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="D30" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="E30" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -4046,13 +4064,13 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="D31" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E31" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -4061,10 +4079,10 @@
         <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E32" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -4073,13 +4091,13 @@
         <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="D33" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="E33" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -4088,10 +4106,10 @@
         <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E34" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -4100,25 +4118,25 @@
         <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E35" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>935</v>
       </c>
       <c r="C36" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="D36" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E36" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -4127,13 +4145,13 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="D37" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="E37" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -4142,10 +4160,10 @@
         <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="E38" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -4154,10 +4172,10 @@
         <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E39" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -4166,13 +4184,13 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="D40" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E40" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -4181,10 +4199,10 @@
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="E41" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -4193,13 +4211,13 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="D42" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E42" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -4208,10 +4226,10 @@
         <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="E43" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -4220,10 +4238,10 @@
         <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E44" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -4232,10 +4250,10 @@
         <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E45" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -4244,13 +4262,13 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="D46" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E46" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -4259,13 +4277,13 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="D47" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E47" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -4274,13 +4292,13 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="D48" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E48" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -4289,13 +4307,13 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="D49" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E49" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -4304,25 +4322,28 @@
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="D50" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="E50" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" t="s">
-        <v>266</v>
+        <v>938</v>
+      </c>
+      <c r="C51" t="s">
+        <v>265</v>
       </c>
       <c r="D51" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E51" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -4331,13 +4352,13 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="D52" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="E52" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -4346,10 +4367,10 @@
         <v>72</v>
       </c>
       <c r="D53" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E53" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -4358,13 +4379,13 @@
         <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="D54" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E54" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -4373,13 +4394,13 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="D55" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E55" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -4388,13 +4409,13 @@
         <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="D56" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E56" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -4403,13 +4424,13 @@
         <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="D57" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E57" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -4418,13 +4439,13 @@
         <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="D58" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="E58" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -4436,10 +4457,10 @@
         <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E59" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -4448,10 +4469,10 @@
         <v>79</v>
       </c>
       <c r="D60" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E60" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -4460,10 +4481,10 @@
         <v>80</v>
       </c>
       <c r="D61" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E61" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -4472,13 +4493,13 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="D62" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E62" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -4487,13 +4508,13 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="D63" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E63" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -4502,13 +4523,13 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="D64" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E64" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -4517,13 +4538,13 @@
         <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="D65" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E65" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4532,13 +4553,13 @@
         <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="D66" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E66" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -4547,13 +4568,13 @@
         <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="D67" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E67" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -4562,10 +4583,10 @@
         <v>87</v>
       </c>
       <c r="D68" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="E68" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -4574,13 +4595,13 @@
         <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="D69" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E69" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4589,13 +4610,13 @@
         <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="D70" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E70" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -4604,13 +4625,13 @@
         <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="D71" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E71" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -4619,13 +4640,13 @@
         <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="D72" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="E72" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -4634,10 +4655,10 @@
         <v>92</v>
       </c>
       <c r="D73" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E73" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -4646,13 +4667,13 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="D74" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E74" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -4661,13 +4682,13 @@
         <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="D75" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="E75" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -4676,13 +4697,13 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="D76" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="E76" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -4691,13 +4712,13 @@
         <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="D77" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E77" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -4706,13 +4727,13 @@
         <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="D78" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E78" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -4721,10 +4742,10 @@
         <v>98</v>
       </c>
       <c r="D79" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="E79" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -4733,13 +4754,13 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="D80" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E80" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -4748,25 +4769,25 @@
         <v>100</v>
       </c>
       <c r="D81" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="E81" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" t="s">
-        <v>267</v>
+        <v>937</v>
       </c>
       <c r="C82" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="D82" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E82" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -4775,13 +4796,13 @@
         <v>101</v>
       </c>
       <c r="C83" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="D83" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E83" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -4790,13 +4811,13 @@
         <v>102</v>
       </c>
       <c r="C84" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="D84" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="E84" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -4805,10 +4826,10 @@
         <v>103</v>
       </c>
       <c r="D85" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E85" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -4817,10 +4838,10 @@
         <v>104</v>
       </c>
       <c r="D86" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E86" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -4829,13 +4850,13 @@
         <v>105</v>
       </c>
       <c r="C87" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="D87" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E87" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -4844,10 +4865,10 @@
         <v>106</v>
       </c>
       <c r="D88" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E88" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -4856,13 +4877,13 @@
         <v>107</v>
       </c>
       <c r="C89" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="D89" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E89" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -4871,10 +4892,10 @@
         <v>108</v>
       </c>
       <c r="D90" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E90" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -4883,13 +4904,13 @@
         <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D91" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E91" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -4898,13 +4919,13 @@
         <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="D92" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E92" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -4913,13 +4934,13 @@
         <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="D93" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="E93" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -4928,13 +4949,13 @@
         <v>112</v>
       </c>
       <c r="C94" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="D94" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="E94" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -4943,10 +4964,10 @@
         <v>113</v>
       </c>
       <c r="D95" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E95" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -4955,10 +4976,10 @@
         <v>114</v>
       </c>
       <c r="D96" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E96" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -4967,13 +4988,13 @@
         <v>115</v>
       </c>
       <c r="C97" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="D97" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="E97" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -4982,10 +5003,10 @@
         <v>116</v>
       </c>
       <c r="D98" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E98" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -4994,10 +5015,10 @@
         <v>117</v>
       </c>
       <c r="D99" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E99" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -5006,13 +5027,13 @@
         <v>118</v>
       </c>
       <c r="C100" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="D100" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="E100" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -5021,13 +5042,13 @@
         <v>119</v>
       </c>
       <c r="C101" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="D101" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="E101" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -5036,10 +5057,10 @@
         <v>120</v>
       </c>
       <c r="D102" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="E102" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -5048,13 +5069,13 @@
         <v>121</v>
       </c>
       <c r="C103" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="D103" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="E103" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -5063,13 +5084,13 @@
         <v>122</v>
       </c>
       <c r="C104" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="D104" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="E104" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -5078,13 +5099,13 @@
         <v>123</v>
       </c>
       <c r="C105" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="D105" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="E105" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -5096,10 +5117,10 @@
         <v>124</v>
       </c>
       <c r="D106" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="E106" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -5108,13 +5129,13 @@
         <v>125</v>
       </c>
       <c r="C107" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="D107" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="E107" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -5123,10 +5144,10 @@
         <v>126</v>
       </c>
       <c r="D108" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="E108" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -5135,13 +5156,13 @@
         <v>127</v>
       </c>
       <c r="C109" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="D109" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="E109" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -5150,10 +5171,10 @@
         <v>128</v>
       </c>
       <c r="D110" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E110" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -5162,25 +5183,25 @@
         <v>129</v>
       </c>
       <c r="D111" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E111" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" t="s">
-        <v>268</v>
+        <v>939</v>
       </c>
       <c r="C112" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="D112" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E112" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -5189,13 +5210,13 @@
         <v>130</v>
       </c>
       <c r="C113" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="D113" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="E113" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -5204,13 +5225,13 @@
         <v>131</v>
       </c>
       <c r="C114" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="D114" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="E114" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -5219,13 +5240,13 @@
         <v>132</v>
       </c>
       <c r="C115" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="D115" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="E115" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -5234,13 +5255,13 @@
         <v>133</v>
       </c>
       <c r="C116" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="D116" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E116" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -5249,10 +5270,10 @@
         <v>134</v>
       </c>
       <c r="D117" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="E117" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -5261,10 +5282,10 @@
         <v>135</v>
       </c>
       <c r="D118" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="E118" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -5273,13 +5294,13 @@
         <v>136</v>
       </c>
       <c r="C119" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="D119" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="E119" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -5288,10 +5309,10 @@
         <v>137</v>
       </c>
       <c r="D120" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="E120" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -5300,13 +5321,13 @@
         <v>138</v>
       </c>
       <c r="C121" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="D121" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E121" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -5315,13 +5336,13 @@
         <v>139</v>
       </c>
       <c r="C122" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="D122" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="E122" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -5330,13 +5351,13 @@
         <v>140</v>
       </c>
       <c r="C123" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="D123" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E123" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -5345,13 +5366,13 @@
         <v>141</v>
       </c>
       <c r="C124" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="D124" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="E124" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -5360,13 +5381,13 @@
         <v>142</v>
       </c>
       <c r="C125" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="D125" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E125" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -5375,22 +5396,25 @@
         <v>143</v>
       </c>
       <c r="D126" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="E126" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" t="s">
-        <v>269</v>
+        <v>940</v>
+      </c>
+      <c r="C127" t="s">
+        <v>266</v>
       </c>
       <c r="D127" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E127" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -5399,25 +5423,28 @@
         <v>144</v>
       </c>
       <c r="C128" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="D128" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="E128" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" t="s">
+        <v>941</v>
+      </c>
+      <c r="C129" t="s">
         <v>145</v>
       </c>
       <c r="D129" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E129" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -5426,13 +5453,13 @@
         <v>146</v>
       </c>
       <c r="C130" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="D130" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="E130" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -5441,13 +5468,13 @@
         <v>147</v>
       </c>
       <c r="C131" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="D131" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E131" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -5459,10 +5486,10 @@
         <v>148</v>
       </c>
       <c r="D132" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="E132" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -5471,10 +5498,10 @@
         <v>149</v>
       </c>
       <c r="D133" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="E133" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -5483,13 +5510,13 @@
         <v>150</v>
       </c>
       <c r="C134" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="D134" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E134" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -5498,13 +5525,13 @@
         <v>151</v>
       </c>
       <c r="C135" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="D135" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E135" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -5513,13 +5540,13 @@
         <v>152</v>
       </c>
       <c r="C136" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="D136" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="E136" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -5528,13 +5555,13 @@
         <v>153</v>
       </c>
       <c r="C137" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="D137" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E137" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -5543,13 +5570,13 @@
         <v>154</v>
       </c>
       <c r="C138" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="D138" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="E138" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -5558,13 +5585,13 @@
         <v>155</v>
       </c>
       <c r="C139" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="D139" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="E139" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -5573,13 +5600,13 @@
         <v>156</v>
       </c>
       <c r="C140" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="D140" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="E140" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -5588,10 +5615,10 @@
         <v>157</v>
       </c>
       <c r="D141" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="E141" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -5600,13 +5627,13 @@
         <v>158</v>
       </c>
       <c r="C142" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="D142" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="E142" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -5615,28 +5642,28 @@
         <v>159</v>
       </c>
       <c r="C143" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="D143" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="E143" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" t="s">
-        <v>270</v>
+        <v>944</v>
       </c>
       <c r="C144" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="D144" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E144" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -5645,13 +5672,13 @@
         <v>160</v>
       </c>
       <c r="C145" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="D145" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E145" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -5660,13 +5687,13 @@
         <v>161</v>
       </c>
       <c r="C146" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="D146" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E146" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -5675,13 +5702,13 @@
         <v>162</v>
       </c>
       <c r="C147" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="D147" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="E147" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -5690,13 +5717,13 @@
         <v>163</v>
       </c>
       <c r="C148" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="D148" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="E148" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -5705,13 +5732,13 @@
         <v>164</v>
       </c>
       <c r="C149" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="D149" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="E149" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -5720,13 +5747,13 @@
         <v>165</v>
       </c>
       <c r="C150" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="D150" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="E150" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -5735,13 +5762,13 @@
         <v>166</v>
       </c>
       <c r="C151" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="D151" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="E151" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -5750,13 +5777,13 @@
         <v>167</v>
       </c>
       <c r="C152" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="D152" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E152" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -5768,10 +5795,10 @@
         <v>168</v>
       </c>
       <c r="D153" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="E153" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -5780,10 +5807,10 @@
         <v>169</v>
       </c>
       <c r="D154" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="E154" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -5792,13 +5819,13 @@
         <v>170</v>
       </c>
       <c r="C155" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="D155" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="E155" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -5807,13 +5834,13 @@
         <v>171</v>
       </c>
       <c r="C156" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="D156" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="E156" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -5822,13 +5849,13 @@
         <v>172</v>
       </c>
       <c r="C157" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="D157" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="E157" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -5837,10 +5864,10 @@
         <v>173</v>
       </c>
       <c r="D158" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="E158" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -5849,10 +5876,10 @@
         <v>174</v>
       </c>
       <c r="D159" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="E159" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -5861,13 +5888,13 @@
         <v>175</v>
       </c>
       <c r="C160" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="D160" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="E160" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -5876,13 +5903,13 @@
         <v>176</v>
       </c>
       <c r="C161" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="D161" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="E161" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -5891,10 +5918,10 @@
         <v>177</v>
       </c>
       <c r="D162" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="E162" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -5903,10 +5930,10 @@
         <v>178</v>
       </c>
       <c r="D163" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="E163" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -5915,13 +5942,13 @@
         <v>179</v>
       </c>
       <c r="C164" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="D164" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="E164" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -5930,10 +5957,10 @@
         <v>180</v>
       </c>
       <c r="D165" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="E165" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -5942,13 +5969,13 @@
         <v>181</v>
       </c>
       <c r="C166" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="D166" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="E166" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -5957,10 +5984,10 @@
         <v>182</v>
       </c>
       <c r="D167" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="E167" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -5969,13 +5996,13 @@
         <v>183</v>
       </c>
       <c r="C168" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="D168" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="E168" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -5984,13 +6011,13 @@
         <v>184</v>
       </c>
       <c r="C169" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="D169" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E169" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6002,10 +6029,10 @@
         <v>185</v>
       </c>
       <c r="D170" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="E170" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -6014,13 +6041,13 @@
         <v>186</v>
       </c>
       <c r="C171" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="D171" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="E171" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -6029,13 +6056,13 @@
         <v>187</v>
       </c>
       <c r="C172" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="D172" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="E172" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -6044,13 +6071,13 @@
         <v>188</v>
       </c>
       <c r="C173" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="D173" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="E173" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -6059,13 +6086,13 @@
         <v>189</v>
       </c>
       <c r="C174" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="D174" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="E174" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -6074,10 +6101,10 @@
         <v>190</v>
       </c>
       <c r="D175" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="E175" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -6086,13 +6113,13 @@
         <v>191</v>
       </c>
       <c r="C176" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="D176" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="E176" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -6101,13 +6128,13 @@
         <v>192</v>
       </c>
       <c r="C177" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="D177" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="E177" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6116,13 +6143,13 @@
         <v>193</v>
       </c>
       <c r="C178" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="D178" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="E178" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -6131,10 +6158,10 @@
         <v>194</v>
       </c>
       <c r="D179" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="E179" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -6143,13 +6170,13 @@
         <v>195</v>
       </c>
       <c r="C180" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="D180" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="E180" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -6158,13 +6185,13 @@
         <v>196</v>
       </c>
       <c r="C181" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="D181" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E181" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -6173,13 +6200,13 @@
         <v>197</v>
       </c>
       <c r="C182" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="D182" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="E182" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -6188,13 +6215,13 @@
         <v>198</v>
       </c>
       <c r="C183" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="D183" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E183" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -6203,13 +6230,13 @@
         <v>199</v>
       </c>
       <c r="C184" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="D184" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="E184" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -6218,25 +6245,25 @@
         <v>200</v>
       </c>
       <c r="D185" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="E185" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" t="s">
-        <v>271</v>
+        <v>942</v>
       </c>
       <c r="C186" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="D186" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="E186" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -6245,13 +6272,13 @@
         <v>201</v>
       </c>
       <c r="C187" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="D187" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="E187" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -6260,28 +6287,28 @@
         <v>202</v>
       </c>
       <c r="C188" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="D188" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E188" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" t="s">
-        <v>272</v>
+        <v>947</v>
       </c>
       <c r="C189" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="D189" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="E189" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -6290,10 +6317,10 @@
         <v>203</v>
       </c>
       <c r="D190" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="E190" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -6302,13 +6329,13 @@
         <v>204</v>
       </c>
       <c r="C191" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="D191" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="E191" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -6317,10 +6344,10 @@
         <v>205</v>
       </c>
       <c r="D192" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="E192" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -6329,10 +6356,10 @@
         <v>206</v>
       </c>
       <c r="D193" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="E193" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -6341,10 +6368,10 @@
         <v>207</v>
       </c>
       <c r="D194" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="E194" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -6353,13 +6380,13 @@
         <v>208</v>
       </c>
       <c r="C195" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="D195" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="E195" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -6368,13 +6395,13 @@
         <v>209</v>
       </c>
       <c r="C196" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="D196" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="E196" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -6383,13 +6410,13 @@
         <v>210</v>
       </c>
       <c r="C197" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="D197" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="E197" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -6398,13 +6425,13 @@
         <v>211</v>
       </c>
       <c r="C198" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="D198" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="E198" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -6413,13 +6440,13 @@
         <v>212</v>
       </c>
       <c r="C199" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D199" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="E199" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -6428,22 +6455,22 @@
         <v>213</v>
       </c>
       <c r="D200" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="E200" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D201" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="E201" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -6452,10 +6479,10 @@
         <v>214</v>
       </c>
       <c r="D202" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="E202" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -6464,10 +6491,10 @@
         <v>215</v>
       </c>
       <c r="D203" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="E203" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -6476,13 +6503,13 @@
         <v>216</v>
       </c>
       <c r="C204" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="D204" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="E204" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -6491,13 +6518,13 @@
         <v>217</v>
       </c>
       <c r="C205" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="D205" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="E205" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -6506,13 +6533,13 @@
         <v>218</v>
       </c>
       <c r="C206" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="D206" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="E206" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -6521,13 +6548,13 @@
         <v>219</v>
       </c>
       <c r="C207" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="D207" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="E207" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -6536,10 +6563,10 @@
         <v>220</v>
       </c>
       <c r="D208" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="E208" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -6548,13 +6575,13 @@
         <v>221</v>
       </c>
       <c r="C209" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="D209" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="E209" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -6563,13 +6590,13 @@
         <v>222</v>
       </c>
       <c r="C210" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="D210" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="E210" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -6578,13 +6605,13 @@
         <v>223</v>
       </c>
       <c r="C211" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="D211" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E211" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -6593,13 +6620,13 @@
         <v>224</v>
       </c>
       <c r="C212" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="D212" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="E212" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -6608,13 +6635,13 @@
         <v>225</v>
       </c>
       <c r="C213" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="D213" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="E213" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -6623,13 +6650,13 @@
         <v>226</v>
       </c>
       <c r="C214" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="D214" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="E214" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -6638,13 +6665,13 @@
         <v>227</v>
       </c>
       <c r="C215" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="D215" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="E215" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
@@ -6653,13 +6680,13 @@
         <v>228</v>
       </c>
       <c r="C216" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="D216" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="E216" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
@@ -6671,10 +6698,10 @@
         <v>229</v>
       </c>
       <c r="D217" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="E217" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
@@ -6683,25 +6710,28 @@
         <v>230</v>
       </c>
       <c r="C218" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D218" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="E218" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" t="s">
+        <v>943</v>
+      </c>
+      <c r="C219" t="s">
         <v>231</v>
       </c>
       <c r="D219" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="E219" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
@@ -6710,10 +6740,10 @@
         <v>232</v>
       </c>
       <c r="D220" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="E220" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
@@ -6722,13 +6752,13 @@
         <v>233</v>
       </c>
       <c r="C221" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="D221" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E221" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
@@ -6737,13 +6767,13 @@
         <v>234</v>
       </c>
       <c r="C222" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="D222" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="E222" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -6752,13 +6782,13 @@
         <v>235</v>
       </c>
       <c r="C223" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="D223" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="E223" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
@@ -6767,13 +6797,13 @@
         <v>236</v>
       </c>
       <c r="C224" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="D224" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E224" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -6782,10 +6812,10 @@
         <v>237</v>
       </c>
       <c r="D225" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="E225" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -6794,10 +6824,10 @@
         <v>238</v>
       </c>
       <c r="D226" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="E226" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
@@ -6806,13 +6836,13 @@
         <v>239</v>
       </c>
       <c r="C227" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="D227" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="E227" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
@@ -6821,13 +6851,13 @@
         <v>240</v>
       </c>
       <c r="C228" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="D228" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="E228" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
@@ -6836,13 +6866,13 @@
         <v>241</v>
       </c>
       <c r="C229" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="D229" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="E229" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
@@ -6851,13 +6881,13 @@
         <v>242</v>
       </c>
       <c r="C230" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="D230" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E230" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
@@ -6866,13 +6896,13 @@
         <v>243</v>
       </c>
       <c r="C231" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="D231" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="E231" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -6881,40 +6911,40 @@
         <v>244</v>
       </c>
       <c r="D232" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="E232" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" t="s">
-        <v>274</v>
+        <v>948</v>
       </c>
       <c r="C233" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D233" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="E233" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" t="s">
-        <v>275</v>
+        <v>945</v>
       </c>
       <c r="C234" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="D234" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E234" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
@@ -6923,13 +6953,13 @@
         <v>245</v>
       </c>
       <c r="C235" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="D235" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="E235" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
@@ -6938,10 +6968,10 @@
         <v>246</v>
       </c>
       <c r="D236" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="E236" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
@@ -6950,10 +6980,10 @@
         <v>247</v>
       </c>
       <c r="D237" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E237" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -6962,13 +6992,13 @@
         <v>248</v>
       </c>
       <c r="C238" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="D238" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="E238" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
@@ -6977,13 +7007,13 @@
         <v>249</v>
       </c>
       <c r="C239" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="D239" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E239" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
@@ -6992,25 +7022,28 @@
         <v>250</v>
       </c>
       <c r="C240" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="D240" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="E240" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" t="s">
+        <v>936</v>
+      </c>
+      <c r="C241" t="s">
         <v>251</v>
       </c>
       <c r="D241" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="E241" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
@@ -7019,55 +7052,55 @@
         <v>252</v>
       </c>
       <c r="D242" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E242" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" t="s">
-        <v>276</v>
+        <v>946</v>
       </c>
       <c r="C243" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="D243" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E243" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C244" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="D244" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="E244" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C245" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="D245" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E245" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
@@ -7076,13 +7109,13 @@
         <v>253</v>
       </c>
       <c r="C246" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="D246" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="E246" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
@@ -7091,13 +7124,13 @@
         <v>254</v>
       </c>
       <c r="C247" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="D247" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E247" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -7106,10 +7139,10 @@
         <v>255</v>
       </c>
       <c r="D248" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E248" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -7118,13 +7151,13 @@
         <v>256</v>
       </c>
       <c r="C249" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="D249" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="E249" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -7133,13 +7166,13 @@
         <v>257</v>
       </c>
       <c r="C250" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="D250" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="E250" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
@@ -7148,13 +7181,13 @@
         <v>258</v>
       </c>
       <c r="C251" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="D251" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="E251" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -7163,13 +7196,13 @@
         <v>259</v>
       </c>
       <c r="C252" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="D252" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="E252" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -7178,13 +7211,13 @@
         <v>260</v>
       </c>
       <c r="C253" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="D253" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="E253" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a general-config feature to add all countries to RegionCodeList (#262)
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52C331-6745-1945-B300-D1256730E721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4961F8-0C7B-A349-A0E4-B102F9455CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" activeTab="2" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="951">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -839,42 +839,18 @@
     <t>Bonaire, Sint Eustatius and Saba</t>
   </si>
   <si>
-    <t>Bolivia, Plurinational State of</t>
-  </si>
-  <si>
     <t>Congo, The Democratic Republic of the</t>
   </si>
   <si>
-    <t>Micronesia, Federated States of</t>
-  </si>
-  <si>
-    <t>Iran, Islamic Republic of</t>
-  </si>
-  <si>
     <t>Korea, Republic of</t>
   </si>
   <si>
-    <t>Moldova, Republic of</t>
-  </si>
-  <si>
-    <t>Korea, Democratic People's Republic of</t>
-  </si>
-  <si>
-    <t>Palestine, State of</t>
-  </si>
-  <si>
     <t>Saint Helena, Ascension and Tristan da Cunha</t>
   </si>
   <si>
     <t>Taiwan, Province of China</t>
   </si>
   <si>
-    <t>Tanzania, United Republic of</t>
-  </si>
-  <si>
-    <t>Venezuela, Bolivarian Republic of</t>
-  </si>
-  <si>
     <t>Virgin Islands, British</t>
   </si>
   <si>
@@ -2871,6 +2847,54 @@
   </si>
   <si>
     <t>Republic of Zimbabwe</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Vatican</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>The Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kosovo (under UNSC res. 1244)</t>
   </si>
 </sst>
 </file>
@@ -3368,7 +3392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57125F9-2A76-4330-8B10-EEE4DD8003C0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3620,9 +3644,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C03D5C-5195-7F40-B34C-39F833F922A1}">
-  <dimension ref="A1:I253"/>
+  <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3650,7 +3674,7 @@
         <v>261</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>262</v>
@@ -3667,13 +3691,13 @@
         <v>90</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>11</v>
@@ -3686,10 +3710,10 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E5" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3698,13 +3722,13 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E6" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3713,13 +3737,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="D7" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="E7" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3728,10 +3752,10 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E8" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3740,10 +3764,10 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E9" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3752,13 +3776,13 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="D10" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E10" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3767,13 +3791,13 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="D11" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="E11" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3782,10 +3806,10 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E12" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3794,13 +3818,13 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="D13" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E13" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,13 +3833,13 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D14" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E14" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3824,10 +3848,10 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E15" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3836,10 +3860,10 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E16" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3848,10 +3872,10 @@
         <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E17" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3860,10 +3884,10 @@
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E18" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3872,10 +3896,10 @@
         <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E19" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3884,13 +3908,13 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="D20" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E20" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3899,13 +3923,13 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="D21" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E21" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3914,13 +3938,13 @@
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="D22" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="E22" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3929,13 +3953,13 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="D23" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E23" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3944,13 +3968,13 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="D24" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E24" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3962,10 +3986,10 @@
         <v>264</v>
       </c>
       <c r="D25" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E25" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3974,10 +3998,10 @@
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E26" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3986,13 +4010,13 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="D27" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E27" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4001,13 +4025,13 @@
         <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="D28" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E28" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4016,13 +4040,13 @@
         <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E29" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -4031,13 +4055,13 @@
         <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="D30" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="E30" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -4046,13 +4070,13 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="D31" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E31" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -4061,10 +4085,10 @@
         <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E32" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -4073,13 +4097,13 @@
         <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="D33" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="E33" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -4088,10 +4112,10 @@
         <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E34" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -4100,25 +4124,25 @@
         <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E35" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>935</v>
       </c>
       <c r="C36" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="D36" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E36" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -4127,13 +4151,13 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="D37" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="E37" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -4142,10 +4166,10 @@
         <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="E38" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -4154,10 +4178,10 @@
         <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E39" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -4166,13 +4190,13 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="D40" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E40" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -4181,10 +4205,10 @@
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="E41" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -4193,13 +4217,13 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="D42" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E42" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -4208,10 +4232,10 @@
         <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="E43" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -4220,10 +4244,10 @@
         <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E44" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -4232,10 +4256,10 @@
         <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E45" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -4244,13 +4268,13 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="D46" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E46" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -4259,13 +4283,13 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="D47" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E47" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -4274,13 +4298,13 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="D48" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E48" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -4289,13 +4313,13 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="D49" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E49" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -4304,25 +4328,28 @@
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="D50" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="E50" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" t="s">
-        <v>266</v>
+        <v>938</v>
+      </c>
+      <c r="C51" t="s">
+        <v>265</v>
       </c>
       <c r="D51" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E51" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -4331,13 +4358,13 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="D52" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="E52" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -4346,10 +4373,10 @@
         <v>72</v>
       </c>
       <c r="D53" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E53" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -4358,13 +4385,13 @@
         <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="D54" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E54" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -4373,13 +4400,13 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="D55" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E55" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -4388,13 +4415,13 @@
         <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="D56" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E56" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -4403,13 +4430,13 @@
         <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="D57" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E57" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -4418,13 +4445,13 @@
         <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="D58" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="E58" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -4436,10 +4463,10 @@
         <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E59" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -4448,10 +4475,10 @@
         <v>79</v>
       </c>
       <c r="D60" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E60" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -4460,10 +4487,10 @@
         <v>80</v>
       </c>
       <c r="D61" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E61" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -4472,13 +4499,13 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="D62" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E62" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -4487,13 +4514,13 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="D63" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E63" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -4502,13 +4529,13 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="D64" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E64" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -4517,13 +4544,13 @@
         <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="D65" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E65" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4532,13 +4559,13 @@
         <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="D66" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E66" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -4547,13 +4574,13 @@
         <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="D67" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E67" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -4562,10 +4589,10 @@
         <v>87</v>
       </c>
       <c r="D68" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="E68" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -4574,13 +4601,13 @@
         <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="D69" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E69" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4589,13 +4616,13 @@
         <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="D70" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E70" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -4604,13 +4631,13 @@
         <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="D71" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E71" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -4619,13 +4646,13 @@
         <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="D72" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="E72" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -4634,10 +4661,10 @@
         <v>92</v>
       </c>
       <c r="D73" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E73" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -4646,13 +4673,13 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="D74" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E74" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -4661,13 +4688,13 @@
         <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="D75" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="E75" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -4676,13 +4703,13 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="D76" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="E76" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -4691,13 +4718,13 @@
         <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="D77" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E77" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -4706,13 +4733,13 @@
         <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="D78" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E78" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -4721,10 +4748,10 @@
         <v>98</v>
       </c>
       <c r="D79" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="E79" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -4733,13 +4760,13 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="D80" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E80" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -4748,25 +4775,25 @@
         <v>100</v>
       </c>
       <c r="D81" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="E81" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" t="s">
-        <v>267</v>
+        <v>937</v>
       </c>
       <c r="C82" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="D82" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E82" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -4775,13 +4802,13 @@
         <v>101</v>
       </c>
       <c r="C83" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="D83" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E83" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -4790,13 +4817,13 @@
         <v>102</v>
       </c>
       <c r="C84" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="D84" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="E84" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -4805,10 +4832,10 @@
         <v>103</v>
       </c>
       <c r="D85" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E85" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -4817,10 +4844,10 @@
         <v>104</v>
       </c>
       <c r="D86" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E86" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -4829,13 +4856,13 @@
         <v>105</v>
       </c>
       <c r="C87" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="D87" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E87" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -4844,10 +4871,10 @@
         <v>106</v>
       </c>
       <c r="D88" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E88" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -4856,13 +4883,13 @@
         <v>107</v>
       </c>
       <c r="C89" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="D89" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E89" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -4871,10 +4898,10 @@
         <v>108</v>
       </c>
       <c r="D90" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E90" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -4883,13 +4910,13 @@
         <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D91" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E91" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -4898,13 +4925,13 @@
         <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="D92" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E92" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -4913,13 +4940,13 @@
         <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="D93" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="E93" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -4928,13 +4955,13 @@
         <v>112</v>
       </c>
       <c r="C94" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="D94" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="E94" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -4943,10 +4970,10 @@
         <v>113</v>
       </c>
       <c r="D95" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E95" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -4955,10 +4982,10 @@
         <v>114</v>
       </c>
       <c r="D96" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E96" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -4967,13 +4994,13 @@
         <v>115</v>
       </c>
       <c r="C97" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="D97" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="E97" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -4982,10 +5009,10 @@
         <v>116</v>
       </c>
       <c r="D98" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E98" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -4994,10 +5021,10 @@
         <v>117</v>
       </c>
       <c r="D99" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E99" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -5006,13 +5033,13 @@
         <v>118</v>
       </c>
       <c r="C100" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="D100" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="E100" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -5021,13 +5048,13 @@
         <v>119</v>
       </c>
       <c r="C101" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="D101" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="E101" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -5036,10 +5063,10 @@
         <v>120</v>
       </c>
       <c r="D102" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="E102" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -5048,13 +5075,13 @@
         <v>121</v>
       </c>
       <c r="C103" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="D103" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="E103" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -5063,13 +5090,13 @@
         <v>122</v>
       </c>
       <c r="C104" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="D104" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="E104" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -5078,13 +5105,13 @@
         <v>123</v>
       </c>
       <c r="C105" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="D105" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="E105" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -5096,10 +5123,10 @@
         <v>124</v>
       </c>
       <c r="D106" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="E106" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -5108,13 +5135,13 @@
         <v>125</v>
       </c>
       <c r="C107" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="D107" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="E107" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -5123,10 +5150,10 @@
         <v>126</v>
       </c>
       <c r="D108" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="E108" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -5135,13 +5162,13 @@
         <v>127</v>
       </c>
       <c r="C109" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="D109" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="E109" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -5150,10 +5177,10 @@
         <v>128</v>
       </c>
       <c r="D110" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E110" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -5162,25 +5189,25 @@
         <v>129</v>
       </c>
       <c r="D111" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E111" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" t="s">
-        <v>268</v>
+        <v>939</v>
       </c>
       <c r="C112" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="D112" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E112" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -5189,13 +5216,13 @@
         <v>130</v>
       </c>
       <c r="C113" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="D113" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="E113" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -5204,13 +5231,13 @@
         <v>131</v>
       </c>
       <c r="C114" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="D114" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="E114" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -5219,13 +5246,13 @@
         <v>132</v>
       </c>
       <c r="C115" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="D115" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="E115" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -5234,13 +5261,13 @@
         <v>133</v>
       </c>
       <c r="C116" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="D116" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E116" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -5249,10 +5276,10 @@
         <v>134</v>
       </c>
       <c r="D117" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="E117" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -5261,10 +5288,10 @@
         <v>135</v>
       </c>
       <c r="D118" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="E118" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -5273,13 +5300,13 @@
         <v>136</v>
       </c>
       <c r="C119" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="D119" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="E119" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -5288,10 +5315,10 @@
         <v>137</v>
       </c>
       <c r="D120" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="E120" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -5300,13 +5327,13 @@
         <v>138</v>
       </c>
       <c r="C121" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="D121" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E121" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -5315,13 +5342,13 @@
         <v>139</v>
       </c>
       <c r="C122" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="D122" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="E122" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -5330,13 +5357,13 @@
         <v>140</v>
       </c>
       <c r="C123" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="D123" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E123" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -5345,13 +5372,13 @@
         <v>141</v>
       </c>
       <c r="C124" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="D124" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="E124" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -5360,13 +5387,13 @@
         <v>142</v>
       </c>
       <c r="C125" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="D125" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E125" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -5375,22 +5402,25 @@
         <v>143</v>
       </c>
       <c r="D126" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="E126" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" t="s">
-        <v>269</v>
+        <v>940</v>
+      </c>
+      <c r="C127" t="s">
+        <v>266</v>
       </c>
       <c r="D127" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E127" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -5399,25 +5429,28 @@
         <v>144</v>
       </c>
       <c r="C128" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="D128" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="E128" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" t="s">
+        <v>941</v>
+      </c>
+      <c r="C129" t="s">
         <v>145</v>
       </c>
       <c r="D129" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E129" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -5426,13 +5459,13 @@
         <v>146</v>
       </c>
       <c r="C130" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="D130" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="E130" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -5441,13 +5474,13 @@
         <v>147</v>
       </c>
       <c r="C131" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="D131" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E131" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -5459,10 +5492,10 @@
         <v>148</v>
       </c>
       <c r="D132" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="E132" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -5471,10 +5504,10 @@
         <v>149</v>
       </c>
       <c r="D133" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="E133" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -5483,13 +5516,13 @@
         <v>150</v>
       </c>
       <c r="C134" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="D134" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E134" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -5498,13 +5531,13 @@
         <v>151</v>
       </c>
       <c r="C135" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="D135" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E135" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -5513,13 +5546,13 @@
         <v>152</v>
       </c>
       <c r="C136" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="D136" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="E136" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -5528,13 +5561,13 @@
         <v>153</v>
       </c>
       <c r="C137" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="D137" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E137" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -5543,13 +5576,13 @@
         <v>154</v>
       </c>
       <c r="C138" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="D138" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="E138" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -5558,13 +5591,13 @@
         <v>155</v>
       </c>
       <c r="C139" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="D139" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="E139" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -5573,13 +5606,13 @@
         <v>156</v>
       </c>
       <c r="C140" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="D140" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="E140" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -5588,10 +5621,10 @@
         <v>157</v>
       </c>
       <c r="D141" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="E141" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -5600,13 +5633,13 @@
         <v>158</v>
       </c>
       <c r="C142" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="D142" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="E142" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -5615,28 +5648,28 @@
         <v>159</v>
       </c>
       <c r="C143" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="D143" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="E143" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" t="s">
-        <v>270</v>
+        <v>944</v>
       </c>
       <c r="C144" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="D144" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E144" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -5645,13 +5678,13 @@
         <v>160</v>
       </c>
       <c r="C145" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="D145" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E145" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -5660,13 +5693,13 @@
         <v>161</v>
       </c>
       <c r="C146" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="D146" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E146" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -5675,13 +5708,13 @@
         <v>162</v>
       </c>
       <c r="C147" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="D147" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="E147" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -5690,13 +5723,13 @@
         <v>163</v>
       </c>
       <c r="C148" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="D148" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="E148" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -5705,13 +5738,13 @@
         <v>164</v>
       </c>
       <c r="C149" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="D149" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="E149" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -5720,13 +5753,13 @@
         <v>165</v>
       </c>
       <c r="C150" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="D150" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="E150" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -5735,13 +5768,13 @@
         <v>166</v>
       </c>
       <c r="C151" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="D151" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="E151" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -5750,13 +5783,13 @@
         <v>167</v>
       </c>
       <c r="C152" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="D152" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E152" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -5768,10 +5801,10 @@
         <v>168</v>
       </c>
       <c r="D153" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="E153" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -5780,10 +5813,10 @@
         <v>169</v>
       </c>
       <c r="D154" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="E154" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -5792,13 +5825,13 @@
         <v>170</v>
       </c>
       <c r="C155" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="D155" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="E155" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -5807,13 +5840,13 @@
         <v>171</v>
       </c>
       <c r="C156" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="D156" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="E156" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -5822,13 +5855,13 @@
         <v>172</v>
       </c>
       <c r="C157" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="D157" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="E157" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -5837,10 +5870,10 @@
         <v>173</v>
       </c>
       <c r="D158" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="E158" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -5849,10 +5882,10 @@
         <v>174</v>
       </c>
       <c r="D159" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="E159" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -5861,13 +5894,13 @@
         <v>175</v>
       </c>
       <c r="C160" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="D160" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="E160" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -5876,13 +5909,13 @@
         <v>176</v>
       </c>
       <c r="C161" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="D161" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="E161" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -5891,10 +5924,10 @@
         <v>177</v>
       </c>
       <c r="D162" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="E162" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -5903,10 +5936,10 @@
         <v>178</v>
       </c>
       <c r="D163" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="E163" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -5915,13 +5948,13 @@
         <v>179</v>
       </c>
       <c r="C164" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="D164" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="E164" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -5930,10 +5963,10 @@
         <v>180</v>
       </c>
       <c r="D165" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="E165" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -5942,13 +5975,13 @@
         <v>181</v>
       </c>
       <c r="C166" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="D166" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="E166" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -5957,10 +5990,10 @@
         <v>182</v>
       </c>
       <c r="D167" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="E167" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -5969,13 +6002,13 @@
         <v>183</v>
       </c>
       <c r="C168" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="D168" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="E168" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -5984,13 +6017,13 @@
         <v>184</v>
       </c>
       <c r="C169" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="D169" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E169" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6002,10 +6035,10 @@
         <v>185</v>
       </c>
       <c r="D170" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="E170" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -6014,13 +6047,13 @@
         <v>186</v>
       </c>
       <c r="C171" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="D171" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="E171" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -6029,13 +6062,13 @@
         <v>187</v>
       </c>
       <c r="C172" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="D172" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="E172" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -6044,13 +6077,13 @@
         <v>188</v>
       </c>
       <c r="C173" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="D173" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="E173" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -6059,13 +6092,13 @@
         <v>189</v>
       </c>
       <c r="C174" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="D174" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="E174" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -6074,10 +6107,10 @@
         <v>190</v>
       </c>
       <c r="D175" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="E175" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -6086,13 +6119,13 @@
         <v>191</v>
       </c>
       <c r="C176" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="D176" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="E176" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -6101,13 +6134,13 @@
         <v>192</v>
       </c>
       <c r="C177" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="D177" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="E177" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6116,13 +6149,13 @@
         <v>193</v>
       </c>
       <c r="C178" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="D178" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="E178" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -6131,10 +6164,10 @@
         <v>194</v>
       </c>
       <c r="D179" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="E179" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -6143,13 +6176,13 @@
         <v>195</v>
       </c>
       <c r="C180" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="D180" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="E180" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -6158,13 +6191,13 @@
         <v>196</v>
       </c>
       <c r="C181" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="D181" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E181" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -6173,13 +6206,13 @@
         <v>197</v>
       </c>
       <c r="C182" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="D182" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="E182" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -6188,13 +6221,13 @@
         <v>198</v>
       </c>
       <c r="C183" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="D183" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E183" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -6203,13 +6236,13 @@
         <v>199</v>
       </c>
       <c r="C184" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="D184" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="E184" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -6218,25 +6251,25 @@
         <v>200</v>
       </c>
       <c r="D185" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="E185" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" t="s">
-        <v>271</v>
+        <v>942</v>
       </c>
       <c r="C186" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="D186" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="E186" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -6245,13 +6278,13 @@
         <v>201</v>
       </c>
       <c r="C187" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="D187" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="E187" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -6260,28 +6293,28 @@
         <v>202</v>
       </c>
       <c r="C188" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="D188" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E188" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" t="s">
-        <v>272</v>
+        <v>947</v>
       </c>
       <c r="C189" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="D189" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="E189" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -6290,10 +6323,10 @@
         <v>203</v>
       </c>
       <c r="D190" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="E190" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -6302,13 +6335,13 @@
         <v>204</v>
       </c>
       <c r="C191" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="D191" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="E191" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -6317,10 +6350,10 @@
         <v>205</v>
       </c>
       <c r="D192" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="E192" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -6329,10 +6362,10 @@
         <v>206</v>
       </c>
       <c r="D193" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="E193" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -6341,10 +6374,10 @@
         <v>207</v>
       </c>
       <c r="D194" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="E194" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -6353,13 +6386,13 @@
         <v>208</v>
       </c>
       <c r="C195" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="D195" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="E195" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -6368,13 +6401,13 @@
         <v>209</v>
       </c>
       <c r="C196" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="D196" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="E196" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -6383,13 +6416,13 @@
         <v>210</v>
       </c>
       <c r="C197" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="D197" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="E197" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -6398,13 +6431,13 @@
         <v>211</v>
       </c>
       <c r="C198" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="D198" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="E198" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -6413,13 +6446,13 @@
         <v>212</v>
       </c>
       <c r="C199" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D199" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="E199" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -6428,22 +6461,22 @@
         <v>213</v>
       </c>
       <c r="D200" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="E200" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D201" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="E201" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -6452,10 +6485,10 @@
         <v>214</v>
       </c>
       <c r="D202" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="E202" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -6464,10 +6497,10 @@
         <v>215</v>
       </c>
       <c r="D203" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="E203" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -6476,13 +6509,13 @@
         <v>216</v>
       </c>
       <c r="C204" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="D204" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="E204" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -6491,13 +6524,13 @@
         <v>217</v>
       </c>
       <c r="C205" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="D205" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="E205" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -6506,13 +6539,13 @@
         <v>218</v>
       </c>
       <c r="C206" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="D206" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="E206" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -6521,13 +6554,13 @@
         <v>219</v>
       </c>
       <c r="C207" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="D207" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="E207" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -6536,10 +6569,10 @@
         <v>220</v>
       </c>
       <c r="D208" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="E208" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -6548,13 +6581,13 @@
         <v>221</v>
       </c>
       <c r="C209" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="D209" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="E209" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -6563,13 +6596,13 @@
         <v>222</v>
       </c>
       <c r="C210" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="D210" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="E210" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -6578,13 +6611,13 @@
         <v>223</v>
       </c>
       <c r="C211" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="D211" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E211" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -6593,13 +6626,13 @@
         <v>224</v>
       </c>
       <c r="C212" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="D212" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="E212" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -6608,13 +6641,13 @@
         <v>225</v>
       </c>
       <c r="C213" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="D213" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="E213" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -6623,13 +6656,13 @@
         <v>226</v>
       </c>
       <c r="C214" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="D214" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="E214" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -6638,13 +6671,13 @@
         <v>227</v>
       </c>
       <c r="C215" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="D215" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="E215" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
@@ -6653,13 +6686,13 @@
         <v>228</v>
       </c>
       <c r="C216" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="D216" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="E216" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
@@ -6671,10 +6704,10 @@
         <v>229</v>
       </c>
       <c r="D217" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="E217" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
@@ -6683,25 +6716,28 @@
         <v>230</v>
       </c>
       <c r="C218" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D218" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="E218" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" t="s">
+        <v>943</v>
+      </c>
+      <c r="C219" t="s">
         <v>231</v>
       </c>
       <c r="D219" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="E219" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
@@ -6710,10 +6746,10 @@
         <v>232</v>
       </c>
       <c r="D220" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="E220" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
@@ -6722,13 +6758,13 @@
         <v>233</v>
       </c>
       <c r="C221" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="D221" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E221" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
@@ -6737,13 +6773,13 @@
         <v>234</v>
       </c>
       <c r="C222" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="D222" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="E222" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -6752,13 +6788,13 @@
         <v>235</v>
       </c>
       <c r="C223" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="D223" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="E223" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
@@ -6767,13 +6803,13 @@
         <v>236</v>
       </c>
       <c r="C224" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="D224" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E224" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -6782,10 +6818,10 @@
         <v>237</v>
       </c>
       <c r="D225" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="E225" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -6794,10 +6830,10 @@
         <v>238</v>
       </c>
       <c r="D226" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="E226" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
@@ -6806,13 +6842,13 @@
         <v>239</v>
       </c>
       <c r="C227" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="D227" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="E227" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
@@ -6821,13 +6857,13 @@
         <v>240</v>
       </c>
       <c r="C228" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="D228" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="E228" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
@@ -6836,13 +6872,13 @@
         <v>241</v>
       </c>
       <c r="C229" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="D229" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="E229" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
@@ -6851,13 +6887,13 @@
         <v>242</v>
       </c>
       <c r="C230" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="D230" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="E230" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
@@ -6866,13 +6902,13 @@
         <v>243</v>
       </c>
       <c r="C231" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="D231" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="E231" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -6881,40 +6917,40 @@
         <v>244</v>
       </c>
       <c r="D232" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="E232" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" t="s">
-        <v>274</v>
+        <v>948</v>
       </c>
       <c r="C233" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D233" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="E233" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" t="s">
-        <v>275</v>
+        <v>945</v>
       </c>
       <c r="C234" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="D234" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E234" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
@@ -6923,13 +6959,13 @@
         <v>245</v>
       </c>
       <c r="C235" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="D235" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="E235" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
@@ -6938,10 +6974,10 @@
         <v>246</v>
       </c>
       <c r="D236" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="E236" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
@@ -6950,10 +6986,10 @@
         <v>247</v>
       </c>
       <c r="D237" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E237" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -6962,13 +6998,13 @@
         <v>248</v>
       </c>
       <c r="C238" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="D238" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="E238" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
@@ -6977,13 +7013,13 @@
         <v>249</v>
       </c>
       <c r="C239" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="D239" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E239" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
@@ -6992,25 +7028,28 @@
         <v>250</v>
       </c>
       <c r="C240" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="D240" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="E240" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" t="s">
+        <v>936</v>
+      </c>
+      <c r="C241" t="s">
         <v>251</v>
       </c>
       <c r="D241" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="E241" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
@@ -7019,55 +7058,55 @@
         <v>252</v>
       </c>
       <c r="D242" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E242" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" t="s">
-        <v>276</v>
+        <v>946</v>
       </c>
       <c r="C243" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="D243" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E243" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C244" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="D244" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="E244" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C245" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="D245" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E245" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
@@ -7076,13 +7115,13 @@
         <v>253</v>
       </c>
       <c r="C246" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="D246" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="E246" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
@@ -7091,13 +7130,13 @@
         <v>254</v>
       </c>
       <c r="C247" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="D247" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E247" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -7106,10 +7145,10 @@
         <v>255</v>
       </c>
       <c r="D248" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E248" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -7118,13 +7157,13 @@
         <v>256</v>
       </c>
       <c r="C249" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="D249" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="E249" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -7133,13 +7172,13 @@
         <v>257</v>
       </c>
       <c r="C250" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="D250" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="E250" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
@@ -7148,13 +7187,13 @@
         <v>258</v>
       </c>
       <c r="C251" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="D251" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="E251" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -7163,13 +7202,13 @@
         <v>259</v>
       </c>
       <c r="C252" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="D252" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="E252" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -7178,13 +7217,22 @@
         <v>260</v>
       </c>
       <c r="C253" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="D253" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="E253" t="s">
-        <v>777</v>
+        <v>769</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" s="1"/>
+      <c r="B254" t="s">
+        <v>949</v>
+      </c>
+      <c r="C254" t="s">
+        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change order of countries, add comment on missing ISO3 code for Kosovo
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4961F8-0C7B-A349-A0E4-B102F9455CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D09555-669A-2546-A71E-577D1C310AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" activeTab="2" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="952">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -2895,6 +2895,9 @@
   </si>
   <si>
     <t>Kosovo (under UNSC res. 1244)</t>
+  </si>
+  <si>
+    <t>Kosovo does not have ISO3/ISO2 codes under ISO 3166-1 because it is not a universally recognized state</t>
   </si>
 </sst>
 </file>
@@ -3392,7 +3395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57125F9-2A76-4330-8B10-EEE4DD8003C0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3646,7 +3649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C03D5C-5195-7F40-B34C-39F833F922A1}">
   <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -5210,7 +5213,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
         <v>130</v>
@@ -5225,7 +5228,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" t="s">
         <v>131</v>
@@ -5240,7 +5243,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" t="s">
         <v>132</v>
@@ -5255,7 +5258,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" t="s">
         <v>133</v>
@@ -5270,7 +5273,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" t="s">
         <v>134</v>
@@ -5282,7 +5285,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" t="s">
         <v>135</v>
@@ -5294,7 +5297,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" t="s">
         <v>136</v>
@@ -5309,7 +5312,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" t="s">
         <v>137</v>
@@ -5321,7 +5324,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" t="s">
         <v>138</v>
@@ -5336,7 +5339,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" t="s">
         <v>139</v>
@@ -5351,1888 +5354,1891 @@
         <v>638</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" t="s">
-        <v>140</v>
+        <v>949</v>
       </c>
       <c r="C123" t="s">
-        <v>843</v>
-      </c>
-      <c r="D123" t="s">
-        <v>390</v>
-      </c>
-      <c r="E123" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+        <v>950</v>
+      </c>
+      <c r="F123" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C124" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D124" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E124" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C125" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D125" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E125" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="C126" t="s">
+        <v>845</v>
       </c>
       <c r="D126" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E126" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" t="s">
-        <v>940</v>
-      </c>
-      <c r="C127" t="s">
-        <v>266</v>
+        <v>143</v>
       </c>
       <c r="D127" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E127" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" t="s">
-        <v>144</v>
+        <v>940</v>
       </c>
       <c r="C128" t="s">
-        <v>846</v>
+        <v>266</v>
       </c>
       <c r="D128" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E128" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" t="s">
-        <v>941</v>
+        <v>144</v>
       </c>
       <c r="C129" t="s">
-        <v>145</v>
+        <v>846</v>
       </c>
       <c r="D129" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E129" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" t="s">
-        <v>146</v>
+        <v>941</v>
       </c>
       <c r="C130" t="s">
-        <v>847</v>
+        <v>145</v>
       </c>
       <c r="D130" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E130" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C131" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C132" t="s">
-        <v>148</v>
+        <v>848</v>
       </c>
       <c r="D132" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E132" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+      <c r="C133" t="s">
+        <v>148</v>
       </c>
       <c r="D133" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E133" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" t="s">
-        <v>150</v>
-      </c>
-      <c r="C134" t="s">
-        <v>849</v>
+        <v>149</v>
       </c>
       <c r="D134" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E134" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C135" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D135" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E135" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C136" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D136" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E136" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C137" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D137" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E137" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C138" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D138" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E138" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C139" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D139" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E139" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C140" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D140" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E140" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+      <c r="C141" t="s">
+        <v>855</v>
       </c>
       <c r="D141" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E141" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" t="s">
-        <v>158</v>
-      </c>
-      <c r="C142" t="s">
-        <v>856</v>
+        <v>157</v>
       </c>
       <c r="D142" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E142" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C143" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D143" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E143" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" t="s">
-        <v>944</v>
+        <v>159</v>
       </c>
       <c r="C144" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D144" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E144" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" t="s">
-        <v>160</v>
+        <v>944</v>
       </c>
       <c r="C145" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D145" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E145" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C146" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D146" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E146" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C147" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D147" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E147" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C148" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D148" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E148" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C149" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D149" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E149" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C150" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D150" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E150" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C151" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D151" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E151" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C152" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D152" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E152" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C153" t="s">
-        <v>168</v>
+        <v>866</v>
       </c>
       <c r="D153" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E153" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="C154" t="s">
+        <v>168</v>
       </c>
       <c r="D154" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E154" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" t="s">
-        <v>170</v>
-      </c>
-      <c r="C155" t="s">
-        <v>867</v>
+        <v>169</v>
       </c>
       <c r="D155" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E155" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C156" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D156" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E156" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C157" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D157" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E157" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="C158" t="s">
+        <v>869</v>
       </c>
       <c r="D158" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E158" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D159" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E159" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" t="s">
-        <v>175</v>
-      </c>
-      <c r="C160" t="s">
-        <v>870</v>
+        <v>174</v>
       </c>
       <c r="D160" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E160" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C161" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D161" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E161" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="C162" t="s">
+        <v>871</v>
       </c>
       <c r="D162" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E162" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D163" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E163" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" t="s">
-        <v>179</v>
-      </c>
-      <c r="C164" t="s">
-        <v>872</v>
+        <v>178</v>
       </c>
       <c r="D164" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E164" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" t="s">
-        <v>180</v>
+        <v>179</v>
+      </c>
+      <c r="C165" t="s">
+        <v>872</v>
       </c>
       <c r="D165" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E165" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" t="s">
-        <v>181</v>
-      </c>
-      <c r="C166" t="s">
-        <v>873</v>
+        <v>180</v>
       </c>
       <c r="D166" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E166" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="C167" t="s">
+        <v>873</v>
       </c>
       <c r="D167" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E167" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" t="s">
-        <v>183</v>
-      </c>
-      <c r="C168" t="s">
-        <v>874</v>
+        <v>182</v>
       </c>
       <c r="D168" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E168" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C169" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D169" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E169" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C170" t="s">
-        <v>185</v>
+        <v>875</v>
       </c>
       <c r="D170" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E170" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C171" t="s">
-        <v>876</v>
+        <v>185</v>
       </c>
       <c r="D171" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E171" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C172" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D172" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E172" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C173" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D173" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E173" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C174" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D174" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E174" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="C175" t="s">
+        <v>879</v>
       </c>
       <c r="D175" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E175" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" t="s">
-        <v>191</v>
-      </c>
-      <c r="C176" t="s">
-        <v>880</v>
+        <v>190</v>
       </c>
       <c r="D176" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E176" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C177" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D177" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E177" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C178" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D178" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E178" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="C179" t="s">
+        <v>882</v>
       </c>
       <c r="D179" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E179" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" t="s">
-        <v>195</v>
-      </c>
-      <c r="C180" t="s">
-        <v>883</v>
+        <v>194</v>
       </c>
       <c r="D180" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E180" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C181" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D181" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E181" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C182" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D182" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E182" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C183" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D183" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E183" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C184" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D184" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E184" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="C185" t="s">
+        <v>887</v>
       </c>
       <c r="D185" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E185" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" t="s">
-        <v>942</v>
-      </c>
-      <c r="C186" t="s">
-        <v>888</v>
+        <v>200</v>
       </c>
       <c r="D186" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E186" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" t="s">
-        <v>201</v>
+        <v>942</v>
       </c>
       <c r="C187" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D187" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E187" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C188" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D188" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E188" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" t="s">
-        <v>947</v>
+        <v>202</v>
       </c>
       <c r="C189" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D189" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E189" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" t="s">
-        <v>203</v>
+        <v>947</v>
+      </c>
+      <c r="C190" t="s">
+        <v>891</v>
       </c>
       <c r="D190" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E190" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" t="s">
-        <v>204</v>
-      </c>
-      <c r="C191" t="s">
-        <v>892</v>
+        <v>203</v>
       </c>
       <c r="D191" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E191" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="C192" t="s">
+        <v>892</v>
       </c>
       <c r="D192" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E192" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D193" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E193" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D194" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E194" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" t="s">
-        <v>208</v>
-      </c>
-      <c r="C195" t="s">
-        <v>893</v>
+        <v>207</v>
       </c>
       <c r="D195" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E195" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="B196" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C196" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D196" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E196" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="B197" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C197" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D197" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E197" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="B198" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C198" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D198" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E198" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="B199" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C199" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D199" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E199" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="B200" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="C200" t="s">
+        <v>897</v>
       </c>
       <c r="D200" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E200" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" t="s">
-        <v>267</v>
+        <v>213</v>
       </c>
       <c r="D201" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E201" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
       <c r="D202" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E202" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="B203" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D203" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E203" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="B204" t="s">
-        <v>216</v>
-      </c>
-      <c r="C204" t="s">
-        <v>898</v>
+        <v>215</v>
       </c>
       <c r="D204" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E204" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="B205" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C205" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D205" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E205" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="B206" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C206" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D206" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E206" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C207" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D207" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E207" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="C208" t="s">
+        <v>901</v>
       </c>
       <c r="D208" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E208" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="B209" t="s">
-        <v>221</v>
-      </c>
-      <c r="C209" t="s">
-        <v>902</v>
+        <v>220</v>
       </c>
       <c r="D209" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E209" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="B210" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C210" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D210" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E210" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="B211" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C211" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D211" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E211" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C212" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D212" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E212" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C213" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D213" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E213" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C214" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D214" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E214" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="B215" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C215" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D215" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E215" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1"/>
       <c r="B216" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C216" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D216" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E216" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1"/>
       <c r="B217" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C217" t="s">
-        <v>229</v>
+        <v>909</v>
       </c>
       <c r="D217" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E217" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1"/>
       <c r="B218" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C218" t="s">
-        <v>910</v>
+        <v>229</v>
       </c>
       <c r="D218" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E218" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" t="s">
-        <v>943</v>
+        <v>230</v>
       </c>
       <c r="C219" t="s">
-        <v>231</v>
+        <v>910</v>
       </c>
       <c r="D219" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E219" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1"/>
       <c r="B220" t="s">
-        <v>232</v>
+        <v>943</v>
+      </c>
+      <c r="C220" t="s">
+        <v>231</v>
       </c>
       <c r="D220" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E220" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1"/>
       <c r="B221" t="s">
-        <v>233</v>
-      </c>
-      <c r="C221" t="s">
-        <v>911</v>
+        <v>232</v>
       </c>
       <c r="D221" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E221" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1"/>
       <c r="B222" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C222" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D222" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E222" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1"/>
       <c r="B223" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C223" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D223" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E223" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="B224" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C224" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D224" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E224" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="C225" t="s">
+        <v>914</v>
       </c>
       <c r="D225" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E225" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="B226" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D226" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E226" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="B227" t="s">
-        <v>239</v>
-      </c>
-      <c r="C227" t="s">
-        <v>915</v>
+        <v>238</v>
       </c>
       <c r="D227" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E227" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1"/>
       <c r="B228" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C228" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D228" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E228" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="B229" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C229" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D229" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E229" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="B230" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C230" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D230" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E230" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="B231" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C231" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D231" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E231" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="B232" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="C232" t="s">
+        <v>919</v>
       </c>
       <c r="D232" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E232" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" t="s">
-        <v>948</v>
-      </c>
-      <c r="C233" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D233" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E233" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="C234" t="s">
-        <v>920</v>
+        <v>268</v>
       </c>
       <c r="D234" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E234" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="B235" t="s">
-        <v>245</v>
+        <v>945</v>
       </c>
       <c r="C235" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D235" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E235" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="B236" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="C236" t="s">
+        <v>921</v>
       </c>
       <c r="D236" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E236" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="B237" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D237" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E237" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1"/>
       <c r="B238" t="s">
-        <v>248</v>
-      </c>
-      <c r="C238" t="s">
-        <v>922</v>
+        <v>247</v>
       </c>
       <c r="D238" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E238" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="B239" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C239" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D239" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E239" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="B240" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C240" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D240" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E240" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" t="s">
-        <v>936</v>
+        <v>250</v>
       </c>
       <c r="C241" t="s">
-        <v>251</v>
+        <v>924</v>
       </c>
       <c r="D241" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E241" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="B242" t="s">
-        <v>252</v>
+        <v>936</v>
+      </c>
+      <c r="C242" t="s">
+        <v>251</v>
       </c>
       <c r="D242" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E242" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" t="s">
-        <v>946</v>
-      </c>
-      <c r="C243" t="s">
-        <v>925</v>
+        <v>252</v>
       </c>
       <c r="D243" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E243" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" t="s">
-        <v>269</v>
+        <v>946</v>
       </c>
       <c r="C244" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D244" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E244" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C245" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D245" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E245" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="B246" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="C246" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D246" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E246" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="B247" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C247" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D247" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E247" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="B248" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="C248" t="s">
+        <v>929</v>
       </c>
       <c r="D248" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E248" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="B249" t="s">
-        <v>256</v>
-      </c>
-      <c r="C249" t="s">
-        <v>930</v>
+        <v>255</v>
       </c>
       <c r="D249" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E249" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="B250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C250" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D250" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E250" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="B251" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C251" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D251" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E251" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="B252" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C252" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D252" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E252" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="B253" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C253" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D253" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E253" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="B254" t="s">
-        <v>949</v>
+        <v>260</v>
       </c>
       <c r="C254" t="s">
-        <v>950</v>
+        <v>934</v>
+      </c>
+      <c r="D254" t="s">
+        <v>520</v>
+      </c>
+      <c r="E254" t="s">
+        <v>769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve the docs of the countries feature (#266)
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4961F8-0C7B-A349-A0E4-B102F9455CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D09555-669A-2546-A71E-577D1C310AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" activeTab="2" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="952">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -2895,6 +2895,9 @@
   </si>
   <si>
     <t>Kosovo (under UNSC res. 1244)</t>
+  </si>
+  <si>
+    <t>Kosovo does not have ISO3/ISO2 codes under ISO 3166-1 because it is not a universally recognized state</t>
   </si>
 </sst>
 </file>
@@ -3392,7 +3395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57125F9-2A76-4330-8B10-EEE4DD8003C0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3646,7 +3649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C03D5C-5195-7F40-B34C-39F833F922A1}">
   <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -5210,7 +5213,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
         <v>130</v>
@@ -5225,7 +5228,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" t="s">
         <v>131</v>
@@ -5240,7 +5243,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" t="s">
         <v>132</v>
@@ -5255,7 +5258,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" t="s">
         <v>133</v>
@@ -5270,7 +5273,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" t="s">
         <v>134</v>
@@ -5282,7 +5285,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" t="s">
         <v>135</v>
@@ -5294,7 +5297,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" t="s">
         <v>136</v>
@@ -5309,7 +5312,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" t="s">
         <v>137</v>
@@ -5321,7 +5324,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" t="s">
         <v>138</v>
@@ -5336,7 +5339,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" t="s">
         <v>139</v>
@@ -5351,1888 +5354,1891 @@
         <v>638</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" t="s">
-        <v>140</v>
+        <v>949</v>
       </c>
       <c r="C123" t="s">
-        <v>843</v>
-      </c>
-      <c r="D123" t="s">
-        <v>390</v>
-      </c>
-      <c r="E123" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+        <v>950</v>
+      </c>
+      <c r="F123" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C124" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D124" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E124" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C125" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D125" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E125" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="C126" t="s">
+        <v>845</v>
       </c>
       <c r="D126" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E126" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" t="s">
-        <v>940</v>
-      </c>
-      <c r="C127" t="s">
-        <v>266</v>
+        <v>143</v>
       </c>
       <c r="D127" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E127" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" t="s">
-        <v>144</v>
+        <v>940</v>
       </c>
       <c r="C128" t="s">
-        <v>846</v>
+        <v>266</v>
       </c>
       <c r="D128" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E128" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" t="s">
-        <v>941</v>
+        <v>144</v>
       </c>
       <c r="C129" t="s">
-        <v>145</v>
+        <v>846</v>
       </c>
       <c r="D129" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E129" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" t="s">
-        <v>146</v>
+        <v>941</v>
       </c>
       <c r="C130" t="s">
-        <v>847</v>
+        <v>145</v>
       </c>
       <c r="D130" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E130" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C131" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E131" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C132" t="s">
-        <v>148</v>
+        <v>848</v>
       </c>
       <c r="D132" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E132" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+      <c r="C133" t="s">
+        <v>148</v>
       </c>
       <c r="D133" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E133" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" t="s">
-        <v>150</v>
-      </c>
-      <c r="C134" t="s">
-        <v>849</v>
+        <v>149</v>
       </c>
       <c r="D134" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E134" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C135" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D135" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E135" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C136" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D136" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E136" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C137" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D137" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E137" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C138" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D138" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E138" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C139" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D139" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E139" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C140" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D140" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E140" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+      <c r="C141" t="s">
+        <v>855</v>
       </c>
       <c r="D141" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E141" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" t="s">
-        <v>158</v>
-      </c>
-      <c r="C142" t="s">
-        <v>856</v>
+        <v>157</v>
       </c>
       <c r="D142" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E142" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C143" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D143" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E143" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" t="s">
-        <v>944</v>
+        <v>159</v>
       </c>
       <c r="C144" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D144" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E144" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" t="s">
-        <v>160</v>
+        <v>944</v>
       </c>
       <c r="C145" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D145" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E145" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C146" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D146" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E146" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C147" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D147" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E147" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C148" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D148" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E148" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C149" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D149" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E149" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C150" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D150" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E150" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C151" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D151" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E151" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C152" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D152" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E152" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C153" t="s">
-        <v>168</v>
+        <v>866</v>
       </c>
       <c r="D153" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E153" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="C154" t="s">
+        <v>168</v>
       </c>
       <c r="D154" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E154" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" t="s">
-        <v>170</v>
-      </c>
-      <c r="C155" t="s">
-        <v>867</v>
+        <v>169</v>
       </c>
       <c r="D155" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E155" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C156" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D156" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E156" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C157" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D157" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E157" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="C158" t="s">
+        <v>869</v>
       </c>
       <c r="D158" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E158" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D159" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E159" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" t="s">
-        <v>175</v>
-      </c>
-      <c r="C160" t="s">
-        <v>870</v>
+        <v>174</v>
       </c>
       <c r="D160" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E160" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C161" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D161" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E161" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="C162" t="s">
+        <v>871</v>
       </c>
       <c r="D162" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E162" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D163" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E163" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" t="s">
-        <v>179</v>
-      </c>
-      <c r="C164" t="s">
-        <v>872</v>
+        <v>178</v>
       </c>
       <c r="D164" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E164" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" t="s">
-        <v>180</v>
+        <v>179</v>
+      </c>
+      <c r="C165" t="s">
+        <v>872</v>
       </c>
       <c r="D165" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E165" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" t="s">
-        <v>181</v>
-      </c>
-      <c r="C166" t="s">
-        <v>873</v>
+        <v>180</v>
       </c>
       <c r="D166" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E166" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="C167" t="s">
+        <v>873</v>
       </c>
       <c r="D167" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E167" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" t="s">
-        <v>183</v>
-      </c>
-      <c r="C168" t="s">
-        <v>874</v>
+        <v>182</v>
       </c>
       <c r="D168" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E168" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C169" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D169" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E169" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C170" t="s">
-        <v>185</v>
+        <v>875</v>
       </c>
       <c r="D170" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E170" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C171" t="s">
-        <v>876</v>
+        <v>185</v>
       </c>
       <c r="D171" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E171" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C172" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D172" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E172" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C173" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D173" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E173" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C174" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D174" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E174" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="C175" t="s">
+        <v>879</v>
       </c>
       <c r="D175" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E175" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" t="s">
-        <v>191</v>
-      </c>
-      <c r="C176" t="s">
-        <v>880</v>
+        <v>190</v>
       </c>
       <c r="D176" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E176" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C177" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D177" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E177" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C178" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D178" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E178" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="C179" t="s">
+        <v>882</v>
       </c>
       <c r="D179" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E179" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" t="s">
-        <v>195</v>
-      </c>
-      <c r="C180" t="s">
-        <v>883</v>
+        <v>194</v>
       </c>
       <c r="D180" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E180" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C181" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D181" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E181" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C182" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D182" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E182" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C183" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D183" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E183" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C184" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D184" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E184" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="C185" t="s">
+        <v>887</v>
       </c>
       <c r="D185" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E185" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" t="s">
-        <v>942</v>
-      </c>
-      <c r="C186" t="s">
-        <v>888</v>
+        <v>200</v>
       </c>
       <c r="D186" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E186" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" t="s">
-        <v>201</v>
+        <v>942</v>
       </c>
       <c r="C187" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D187" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E187" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C188" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D188" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E188" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" t="s">
-        <v>947</v>
+        <v>202</v>
       </c>
       <c r="C189" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D189" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E189" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" t="s">
-        <v>203</v>
+        <v>947</v>
+      </c>
+      <c r="C190" t="s">
+        <v>891</v>
       </c>
       <c r="D190" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E190" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" t="s">
-        <v>204</v>
-      </c>
-      <c r="C191" t="s">
-        <v>892</v>
+        <v>203</v>
       </c>
       <c r="D191" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E191" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="C192" t="s">
+        <v>892</v>
       </c>
       <c r="D192" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E192" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D193" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E193" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D194" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E194" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" t="s">
-        <v>208</v>
-      </c>
-      <c r="C195" t="s">
-        <v>893</v>
+        <v>207</v>
       </c>
       <c r="D195" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E195" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="B196" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C196" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D196" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E196" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="B197" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C197" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D197" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E197" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="B198" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C198" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D198" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E198" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="B199" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C199" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D199" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E199" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="B200" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="C200" t="s">
+        <v>897</v>
       </c>
       <c r="D200" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E200" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" t="s">
-        <v>267</v>
+        <v>213</v>
       </c>
       <c r="D201" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E201" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
       <c r="D202" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E202" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="B203" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D203" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E203" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="B204" t="s">
-        <v>216</v>
-      </c>
-      <c r="C204" t="s">
-        <v>898</v>
+        <v>215</v>
       </c>
       <c r="D204" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E204" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="B205" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C205" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D205" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E205" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="B206" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C206" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D206" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E206" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C207" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D207" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E207" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="C208" t="s">
+        <v>901</v>
       </c>
       <c r="D208" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E208" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="B209" t="s">
-        <v>221</v>
-      </c>
-      <c r="C209" t="s">
-        <v>902</v>
+        <v>220</v>
       </c>
       <c r="D209" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E209" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="B210" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C210" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D210" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E210" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="B211" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C211" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D211" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E211" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C212" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D212" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E212" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C213" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D213" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E213" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C214" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D214" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E214" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="B215" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C215" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D215" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E215" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1"/>
       <c r="B216" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C216" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D216" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E216" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1"/>
       <c r="B217" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C217" t="s">
-        <v>229</v>
+        <v>909</v>
       </c>
       <c r="D217" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E217" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1"/>
       <c r="B218" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C218" t="s">
-        <v>910</v>
+        <v>229</v>
       </c>
       <c r="D218" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E218" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" t="s">
-        <v>943</v>
+        <v>230</v>
       </c>
       <c r="C219" t="s">
-        <v>231</v>
+        <v>910</v>
       </c>
       <c r="D219" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E219" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1"/>
       <c r="B220" t="s">
-        <v>232</v>
+        <v>943</v>
+      </c>
+      <c r="C220" t="s">
+        <v>231</v>
       </c>
       <c r="D220" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E220" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1"/>
       <c r="B221" t="s">
-        <v>233</v>
-      </c>
-      <c r="C221" t="s">
-        <v>911</v>
+        <v>232</v>
       </c>
       <c r="D221" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E221" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1"/>
       <c r="B222" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C222" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D222" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E222" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1"/>
       <c r="B223" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C223" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D223" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E223" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="B224" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C224" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D224" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E224" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="C225" t="s">
+        <v>914</v>
       </c>
       <c r="D225" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E225" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="B226" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D226" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E226" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="B227" t="s">
-        <v>239</v>
-      </c>
-      <c r="C227" t="s">
-        <v>915</v>
+        <v>238</v>
       </c>
       <c r="D227" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E227" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1"/>
       <c r="B228" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C228" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D228" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E228" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="B229" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C229" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D229" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E229" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="B230" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C230" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D230" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E230" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="B231" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C231" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D231" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E231" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="B232" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="C232" t="s">
+        <v>919</v>
       </c>
       <c r="D232" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E232" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" t="s">
-        <v>948</v>
-      </c>
-      <c r="C233" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D233" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E233" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="C234" t="s">
-        <v>920</v>
+        <v>268</v>
       </c>
       <c r="D234" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E234" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="B235" t="s">
-        <v>245</v>
+        <v>945</v>
       </c>
       <c r="C235" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D235" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E235" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="B236" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="C236" t="s">
+        <v>921</v>
       </c>
       <c r="D236" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E236" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="B237" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D237" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E237" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1"/>
       <c r="B238" t="s">
-        <v>248</v>
-      </c>
-      <c r="C238" t="s">
-        <v>922</v>
+        <v>247</v>
       </c>
       <c r="D238" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E238" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="B239" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C239" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D239" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E239" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="B240" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C240" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D240" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E240" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" t="s">
-        <v>936</v>
+        <v>250</v>
       </c>
       <c r="C241" t="s">
-        <v>251</v>
+        <v>924</v>
       </c>
       <c r="D241" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E241" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="B242" t="s">
-        <v>252</v>
+        <v>936</v>
+      </c>
+      <c r="C242" t="s">
+        <v>251</v>
       </c>
       <c r="D242" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E242" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" t="s">
-        <v>946</v>
-      </c>
-      <c r="C243" t="s">
-        <v>925</v>
+        <v>252</v>
       </c>
       <c r="D243" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E243" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" t="s">
-        <v>269</v>
+        <v>946</v>
       </c>
       <c r="C244" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D244" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E244" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C245" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D245" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E245" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="B246" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="C246" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D246" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E246" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="B247" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C247" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D247" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E247" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="B248" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="C248" t="s">
+        <v>929</v>
       </c>
       <c r="D248" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E248" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="B249" t="s">
-        <v>256</v>
-      </c>
-      <c r="C249" t="s">
-        <v>930</v>
+        <v>255</v>
       </c>
       <c r="D249" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E249" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="B250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C250" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D250" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E250" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="B251" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C251" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D251" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E251" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="B252" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C252" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D252" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E252" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="B253" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C253" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D253" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E253" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="B254" t="s">
-        <v>949</v>
+        <v>260</v>
       </c>
       <c r="C254" t="s">
-        <v>950</v>
+        <v>934</v>
+      </c>
+      <c r="D254" t="s">
+        <v>520</v>
+      </c>
+      <c r="E254" t="s">
+        <v>769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add preliminary alpha3 code for Kosovo (#373)
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D09555-669A-2546-A71E-577D1C310AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FB7E85-950C-CF44-AB46-C87C68CDFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16520" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="16500" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="953">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -2897,7 +2897,10 @@
     <t>Kosovo (under UNSC res. 1244)</t>
   </si>
   <si>
-    <t>Kosovo does not have ISO3/ISO2 codes under ISO 3166-1 because it is not a universally recognized state</t>
+    <t>KOS</t>
+  </si>
+  <si>
+    <t>Kosovo does not have ISO3/ISO2 codes under ISO 3166-1, this list follows the IOC convention (https://olympics.com/ioc/kosovo)</t>
   </si>
 </sst>
 </file>
@@ -3097,9 +3100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3137,7 +3140,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3243,7 +3246,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3385,7 +3388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5362,8 +5365,11 @@
       <c r="C123" t="s">
         <v>950</v>
       </c>
+      <c r="E123" t="s">
+        <v>951</v>
+      </c>
       <c r="F123" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Sort country list in model registration template
</commit_message>
<xml_diff>
--- a/templates/model-registration-template.xlsx
+++ b/templates/model-registration-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/GitHub/nomenclature/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD035DCB-76D5-9944-8567-F3639F6450E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BCB440-01FB-EC40-934A-83D1E85917DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="16440" windowHeight="16500" xr2:uid="{B27ADFE5-7D44-4C55-83A5-0BFB86B83D12}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="948">
   <si>
     <t xml:space="preserve">Please fill in the cells highlighted with yellow. </t>
     <phoneticPr fontId="1"/>
@@ -2883,6 +2883,9 @@
   </si>
   <si>
     <t>Kosovo does not have officially approved ISO 3166-1 codes, this list follows the conventions by the IOC (https://olympics.com/ioc/kosovo) and Wikipedia (https://en.wikipedia.org/wiki/XK_(user_assigned_code))</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -3671,6 +3674,9 @@
       <c r="E3" s="8" t="s">
         <v>260</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>947</v>
+      </c>
     </row>
     <row r="4" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -3696,511 +3702,511 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>27</v>
+        <v>764</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>764</v>
+        <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="13" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>30</v>
+        <v>802</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>269</v>
+        <v>330</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>518</v>
+        <v>579</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>768</v>
+        <v>38</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>769</v>
+        <v>40</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>37</v>
+        <v>768</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>38</v>
+        <v>769</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>41</v>
+        <v>770</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="13" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>531</v>
+        <v>540</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="13" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="13" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>774</v>
+        <v>58</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>534</v>
+        <v>548</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="13" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>261</v>
+        <v>780</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>47</v>
+        <v>773</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>775</v>
+        <v>55</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="13" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>777</v>
+        <v>56</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>540</v>
+        <v>550</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="13" t="s">
-        <v>52</v>
+        <v>927</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="13" t="s">
-        <v>53</v>
+        <v>261</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>53</v>
+        <v>261</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="13" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>55</v>
+        <v>784</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="13" t="s">
-        <v>927</v>
+        <v>57</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="13" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>782</v>
+        <v>128</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>298</v>
+        <v>370</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>547</v>
+        <v>619</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="13" t="s">
-        <v>58</v>
+        <v>918</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>58</v>
+        <v>918</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>299</v>
+        <v>504</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>548</v>
+        <v>753</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -4221,211 +4227,211 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="13" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="13" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="13" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>784</v>
+        <v>772</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="13" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>63</v>
+        <v>793</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>553</v>
+        <v>566</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="13" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>64</v>
+        <v>837</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>305</v>
+        <v>384</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>554</v>
+        <v>633</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>65</v>
+        <v>789</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>785</v>
+        <v>64</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="13" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>786</v>
+        <v>80</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>787</v>
+        <v>63</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="13" t="s">
-        <v>69</v>
+        <v>231</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>788</v>
+        <v>904</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>310</v>
+        <v>481</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>559</v>
+        <v>730</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="13" t="s">
-        <v>942</v>
+        <v>68</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>942</v>
+        <v>787</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="13" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>790</v>
+        <v>79</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -4461,211 +4467,211 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>794</v>
+        <v>72</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>78</v>
+        <v>788</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="13" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>79</v>
+        <v>824</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>321</v>
+        <v>364</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>570</v>
+        <v>613</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>80</v>
+        <v>795</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>796</v>
+        <v>78</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="13" t="s">
-        <v>84</v>
+        <v>942</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>799</v>
+        <v>942</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>87</v>
+        <v>800</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>802</v>
+        <v>87</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4701,46 +4707,46 @@
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="13" t="s">
-        <v>91</v>
+        <v>216</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>804</v>
+        <v>892</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>332</v>
+        <v>465</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>581</v>
+        <v>714</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="13" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>92</v>
+        <v>818</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>582</v>
+        <v>602</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -4761,316 +4767,316 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="13" t="s">
-        <v>95</v>
+        <v>227</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>807</v>
+        <v>902</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>336</v>
+        <v>476</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>585</v>
+        <v>725</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>809</v>
+        <v>98</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>100</v>
+        <v>808</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="13" t="s">
-        <v>929</v>
+        <v>99</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="13" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>812</v>
+        <v>116</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>592</v>
+        <v>607</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="13" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>813</v>
+        <v>202</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>344</v>
+        <v>450</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>593</v>
+        <v>699</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="13" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>345</v>
+        <v>278</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>594</v>
+        <v>527</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>104</v>
+        <v>812</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="13" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>815</v>
+        <v>798</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>598</v>
+        <v>574</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>108</v>
+        <v>814</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>816</v>
+        <v>106</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>818</v>
+        <v>114</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>819</v>
+        <v>113</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="13" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -5091,121 +5097,121 @@
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="13" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="13" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>117</v>
+        <v>815</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="13" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>120</v>
+        <v>825</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>823</v>
+        <v>120</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -5226,169 +5232,169 @@
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="13" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>616</v>
+        <v>623</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>126</v>
+        <v>827</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="13" t="s">
-        <v>128</v>
+        <v>930</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>128</v>
+        <v>828</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>129</v>
+        <v>829</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="13" t="s">
-        <v>930</v>
+        <v>129</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>828</v>
+        <v>129</v>
       </c>
       <c r="D112" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>829</v>
+        <v>126</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D114" s="13" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>832</v>
+        <v>134</v>
       </c>
       <c r="D116" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="13" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D117" s="13" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="13" t="s">
         <v>135</v>
@@ -5403,7 +5409,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="13" t="s">
         <v>136</v>
@@ -5418,409 +5424,412 @@
         <v>628</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>137</v>
+        <v>834</v>
       </c>
       <c r="D120" s="13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="D122" s="13" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="13" t="s">
-        <v>140</v>
+        <v>940</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>836</v>
+        <v>940</v>
       </c>
       <c r="D123" s="13" t="s">
-        <v>383</v>
+        <v>941</v>
       </c>
       <c r="E123" s="13" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+        <v>945</v>
+      </c>
+      <c r="F123" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="13" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="D124" s="13" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="E124" s="13" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D125" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E125" s="13" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="13" t="s">
-        <v>143</v>
+        <v>932</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>143</v>
+        <v>932</v>
       </c>
       <c r="D126" s="13" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="E126" s="13" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="13" t="s">
-        <v>931</v>
+        <v>154</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>931</v>
+        <v>847</v>
       </c>
       <c r="D127" s="13" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="E127" s="13" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="D128" s="13" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="13" t="s">
-        <v>932</v>
+        <v>151</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>932</v>
+        <v>844</v>
       </c>
       <c r="D129" s="13" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>638</v>
+        <v>645</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="D130" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E130" s="13" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>841</v>
+        <v>147</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E131" s="13" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>147</v>
+        <v>842</v>
       </c>
       <c r="D132" s="13" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E132" s="13" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="13" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>148</v>
+        <v>845</v>
       </c>
       <c r="D133" s="13" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="E133" s="13" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="13" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="D134" s="13" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="E134" s="13" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="13" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="E135" s="13" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="13" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C136" s="13" t="s">
-        <v>844</v>
+        <v>852</v>
       </c>
       <c r="D136" s="13" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="E136" s="13" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="13" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="C137" s="13" t="s">
-        <v>845</v>
+        <v>864</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="E137" s="13" t="s">
-        <v>646</v>
+        <v>670</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="13" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>846</v>
+        <v>176</v>
       </c>
       <c r="D138" s="13" t="s">
-        <v>398</v>
+        <v>422</v>
       </c>
       <c r="E138" s="13" t="s">
-        <v>647</v>
+        <v>671</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="13" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C139" s="13" t="s">
-        <v>847</v>
+        <v>853</v>
       </c>
       <c r="D139" s="13" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="E139" s="13" t="s">
-        <v>648</v>
+        <v>655</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="13" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>848</v>
+        <v>857</v>
       </c>
       <c r="D140" s="13" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="E140" s="13" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="13" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C141" s="13" t="s">
-        <v>156</v>
+        <v>858</v>
       </c>
       <c r="D141" s="13" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="E141" s="13" t="s">
-        <v>650</v>
+        <v>660</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="13" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C142" s="13" t="s">
-        <v>849</v>
+        <v>855</v>
       </c>
       <c r="D142" s="13" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="E142" s="13" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="13" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="C143" s="13" t="s">
-        <v>850</v>
+        <v>173</v>
       </c>
       <c r="D143" s="13" t="s">
-        <v>403</v>
+        <v>419</v>
       </c>
       <c r="E143" s="13" t="s">
-        <v>652</v>
+        <v>668</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="13" t="s">
-        <v>935</v>
+        <v>171</v>
       </c>
       <c r="C144" s="13" t="s">
-        <v>851</v>
+        <v>862</v>
       </c>
       <c r="D144" s="13" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="E144" s="13" t="s">
-        <v>653</v>
+        <v>666</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="13" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>852</v>
+        <v>863</v>
       </c>
       <c r="D145" s="13" t="s">
-        <v>405</v>
+        <v>420</v>
       </c>
       <c r="E145" s="13" t="s">
-        <v>654</v>
+        <v>669</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="13" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="C146" s="13" t="s">
-        <v>853</v>
+        <v>177</v>
       </c>
       <c r="D146" s="13" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="E146" s="13" t="s">
-        <v>655</v>
+        <v>672</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -5841,286 +5850,286 @@
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="13" t="s">
-        <v>162</v>
+        <v>929</v>
       </c>
       <c r="C148" s="13" t="s">
-        <v>855</v>
+        <v>811</v>
       </c>
       <c r="D148" s="13" t="s">
-        <v>408</v>
+        <v>342</v>
       </c>
       <c r="E148" s="13" t="s">
-        <v>657</v>
+        <v>591</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="13" t="s">
-        <v>163</v>
+        <v>935</v>
       </c>
       <c r="C149" s="13" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="D149" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="E149" s="13" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="13" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C150" s="13" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="D150" s="13" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="E150" s="13" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" s="13" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>858</v>
+        <v>168</v>
       </c>
       <c r="D151" s="13" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="E151" s="13" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" s="13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C152" s="13" t="s">
-        <v>859</v>
+        <v>167</v>
       </c>
       <c r="D152" s="13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E152" s="13" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" s="13" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C153" s="13" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D153" s="13" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="E153" s="13" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" s="13" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>168</v>
+        <v>849</v>
       </c>
       <c r="D154" s="13" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="E154" s="13" t="s">
-        <v>663</v>
+        <v>651</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" s="13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C155" s="13" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D155" s="13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E155" s="13" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C156" s="13" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D156" s="13" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E156" s="13" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="13" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="D157" s="13" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="E157" s="13" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" s="13" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C158" s="13" t="s">
-        <v>172</v>
+        <v>872</v>
       </c>
       <c r="D158" s="13" t="s">
-        <v>418</v>
+        <v>434</v>
       </c>
       <c r="E158" s="13" t="s">
-        <v>667</v>
+        <v>683</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" s="13" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C159" s="13" t="s">
-        <v>173</v>
+        <v>871</v>
       </c>
       <c r="D159" s="13" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="E159" s="13" t="s">
-        <v>668</v>
+        <v>682</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" s="13" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>863</v>
+        <v>869</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="E160" s="13" t="s">
-        <v>669</v>
+        <v>680</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C161" s="13" t="s">
-        <v>864</v>
+        <v>179</v>
       </c>
       <c r="D161" s="13" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="E161" s="13" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" s="13" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="D162" s="13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="E162" s="13" t="s">
-        <v>671</v>
+        <v>684</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" s="13" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>177</v>
+        <v>868</v>
       </c>
       <c r="D163" s="13" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="E163" s="13" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" s="13" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D164" s="13" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E164" s="13" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" s="13" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>179</v>
+        <v>867</v>
       </c>
       <c r="D165" s="13" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="E165" s="13" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" s="13" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>866</v>
+        <v>184</v>
       </c>
       <c r="D166" s="13" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="E166" s="13" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -6141,541 +6150,541 @@
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="13" t="s">
-        <v>182</v>
+        <v>933</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>867</v>
+        <v>881</v>
       </c>
       <c r="D168" s="13" t="s">
-        <v>428</v>
+        <v>446</v>
       </c>
       <c r="E168" s="13" t="s">
-        <v>677</v>
+        <v>695</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="13" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>868</v>
+        <v>856</v>
       </c>
       <c r="D169" s="13" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="E169" s="13" t="s">
-        <v>678</v>
+        <v>658</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="13" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>184</v>
+        <v>860</v>
       </c>
       <c r="D170" s="13" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="E170" s="13" t="s">
-        <v>679</v>
+        <v>664</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D171" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E171" s="13" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="13" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="D172" s="13" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="E172" s="13" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" s="13" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="D173" s="13" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="E173" s="13" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" s="13" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c r="D174" s="13" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="E174" s="13" t="s">
-        <v>683</v>
+        <v>691</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" s="13" t="s">
-        <v>189</v>
+        <v>938</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>189</v>
+        <v>884</v>
       </c>
       <c r="D175" s="13" t="s">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="E175" s="13" t="s">
-        <v>684</v>
+        <v>698</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" s="13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C176" s="13" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="D176" s="13" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E176" s="13" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" s="13" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="D177" s="13" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="E177" s="13" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" s="13" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>875</v>
+        <v>883</v>
       </c>
       <c r="D178" s="13" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="E178" s="13" t="s">
-        <v>687</v>
+        <v>697</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>193</v>
+        <v>876</v>
       </c>
       <c r="D179" s="13" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E179" s="13" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D180" s="13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E180" s="13" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C181" s="13" t="s">
-        <v>877</v>
+        <v>193</v>
       </c>
       <c r="D181" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E181" s="13" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" s="13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C182" s="13" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="D182" s="13" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E182" s="13" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" s="13" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="D183" s="13" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="E183" s="13" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C184" s="13" t="s">
-        <v>880</v>
+        <v>199</v>
       </c>
       <c r="D184" s="13" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E184" s="13" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" s="13" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>199</v>
+        <v>885</v>
       </c>
       <c r="D185" s="13" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="E185" s="13" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" s="13" t="s">
-        <v>933</v>
+        <v>204</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>881</v>
+        <v>204</v>
       </c>
       <c r="D186" s="13" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="E186" s="13" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" s="13" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C187" s="13" t="s">
-        <v>882</v>
+        <v>205</v>
       </c>
       <c r="D187" s="13" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="E187" s="13" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" s="13" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>883</v>
+        <v>206</v>
       </c>
       <c r="D188" s="13" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="E188" s="13" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" s="13" t="s">
-        <v>938</v>
+        <v>207</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="D189" s="13" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="E189" s="13" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" s="13" t="s">
-        <v>202</v>
+        <v>53</v>
       </c>
       <c r="C190" s="13" t="s">
-        <v>202</v>
+        <v>53</v>
       </c>
       <c r="D190" s="13" t="s">
-        <v>450</v>
+        <v>293</v>
       </c>
       <c r="E190" s="13" t="s">
-        <v>699</v>
+        <v>542</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" s="13" t="s">
-        <v>203</v>
+        <v>262</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>885</v>
+        <v>262</v>
       </c>
       <c r="D191" s="13" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="E191" s="13" t="s">
-        <v>700</v>
+        <v>710</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" s="13" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="D192" s="13" t="s">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="E192" s="13" t="s">
-        <v>701</v>
+        <v>635</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" s="13" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
       <c r="D193" s="13" t="s">
-        <v>453</v>
+        <v>393</v>
       </c>
       <c r="E193" s="13" t="s">
-        <v>702</v>
+        <v>642</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" s="13" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="D194" s="13" t="s">
-        <v>454</v>
+        <v>401</v>
       </c>
       <c r="E194" s="13" t="s">
-        <v>703</v>
+        <v>650</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" s="13" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>886</v>
+        <v>219</v>
       </c>
       <c r="D195" s="13" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="E195" s="13" t="s">
-        <v>704</v>
+        <v>717</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="B196" s="13" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>887</v>
+        <v>249</v>
       </c>
       <c r="D196" s="13" t="s">
-        <v>456</v>
+        <v>502</v>
       </c>
       <c r="E196" s="13" t="s">
-        <v>705</v>
+        <v>751</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="B197" s="13" t="s">
-        <v>209</v>
+        <v>253</v>
       </c>
       <c r="C197" s="13" t="s">
-        <v>888</v>
+        <v>922</v>
       </c>
       <c r="D197" s="13" t="s">
-        <v>457</v>
+        <v>509</v>
       </c>
       <c r="E197" s="13" t="s">
-        <v>706</v>
+        <v>758</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="B198" s="13" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C198" s="13" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="D198" s="13" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="E198" s="13" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="B199" s="13" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>890</v>
+        <v>897</v>
       </c>
       <c r="D199" s="13" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="E199" s="13" t="s">
-        <v>708</v>
+        <v>720</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="B200" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C200" s="13" t="s">
-        <v>212</v>
+        <v>887</v>
       </c>
       <c r="D200" s="13" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E200" s="13" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" s="13" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="C201" s="13" t="s">
-        <v>262</v>
+        <v>889</v>
       </c>
       <c r="D201" s="13" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E201" s="13" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" s="13" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C202" s="13" t="s">
-        <v>213</v>
+        <v>895</v>
       </c>
       <c r="D202" s="13" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="E202" s="13" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="B203" s="13" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="C203" s="13" t="s">
-        <v>214</v>
+        <v>903</v>
       </c>
       <c r="D203" s="13" t="s">
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="E203" s="13" t="s">
-        <v>712</v>
+        <v>727</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -6696,286 +6705,286 @@
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="B205" s="13" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D205" s="13" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="E205" s="13" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="B206" s="13" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="C206" s="13" t="s">
-        <v>893</v>
+        <v>228</v>
       </c>
       <c r="D206" s="13" t="s">
-        <v>466</v>
+        <v>477</v>
       </c>
       <c r="E206" s="13" t="s">
-        <v>715</v>
+        <v>726</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" s="13" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C207" s="13" t="s">
-        <v>894</v>
+        <v>899</v>
       </c>
       <c r="D207" s="13" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E207" s="13" t="s">
-        <v>716</v>
+        <v>722</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" s="13" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C208" s="13" t="s">
-        <v>219</v>
+        <v>900</v>
       </c>
       <c r="D208" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="E208" s="13" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="B209" s="13" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>895</v>
+        <v>214</v>
       </c>
       <c r="D209" s="13" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E209" s="13" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="B210" s="13" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C210" s="13" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D210" s="13" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E210" s="13" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="B211" s="13" t="s">
-        <v>222</v>
+        <v>255</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>897</v>
+        <v>924</v>
       </c>
       <c r="D211" s="13" t="s">
-        <v>471</v>
+        <v>511</v>
       </c>
       <c r="E211" s="13" t="s">
-        <v>720</v>
+        <v>760</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" s="13" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C212" s="13" t="s">
-        <v>898</v>
+        <v>212</v>
       </c>
       <c r="D212" s="13" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="E212" s="13" t="s">
-        <v>721</v>
+        <v>709</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" s="13" t="s">
-        <v>224</v>
+        <v>931</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>899</v>
+        <v>931</v>
       </c>
       <c r="D213" s="13" t="s">
-        <v>473</v>
+        <v>387</v>
       </c>
       <c r="E213" s="13" t="s">
-        <v>722</v>
+        <v>636</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="D214" s="13" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="E214" s="13" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="B215" s="13" t="s">
-        <v>226</v>
+        <v>93</v>
       </c>
       <c r="C215" s="13" t="s">
-        <v>901</v>
+        <v>805</v>
       </c>
       <c r="D215" s="13" t="s">
-        <v>475</v>
+        <v>334</v>
       </c>
       <c r="E215" s="13" t="s">
-        <v>724</v>
+        <v>583</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1"/>
       <c r="B216" s="13" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>902</v>
+        <v>843</v>
       </c>
       <c r="D216" s="13" t="s">
-        <v>476</v>
+        <v>395</v>
       </c>
       <c r="E216" s="13" t="s">
-        <v>725</v>
+        <v>644</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1"/>
       <c r="B217" s="13" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>228</v>
+        <v>888</v>
       </c>
       <c r="D217" s="13" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="E217" s="13" t="s">
-        <v>726</v>
+        <v>706</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1"/>
       <c r="B218" s="13" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C218" s="13" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="D218" s="13" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E218" s="13" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" s="13" t="s">
-        <v>934</v>
+        <v>213</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>934</v>
+        <v>213</v>
       </c>
       <c r="D219" s="13" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="E219" s="13" t="s">
-        <v>728</v>
+        <v>711</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1"/>
       <c r="B220" s="13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>230</v>
+        <v>901</v>
       </c>
       <c r="D220" s="13" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="E220" s="13" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1"/>
       <c r="B221" s="13" t="s">
-        <v>231</v>
+        <v>66</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>904</v>
+        <v>785</v>
       </c>
       <c r="D221" s="13" t="s">
-        <v>481</v>
+        <v>307</v>
       </c>
       <c r="E221" s="13" t="s">
-        <v>730</v>
+        <v>556</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1"/>
       <c r="B222" s="13" t="s">
-        <v>232</v>
+        <v>934</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>905</v>
+        <v>934</v>
       </c>
       <c r="D222" s="13" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E222" s="13" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1"/>
       <c r="B223" s="13" t="s">
-        <v>233</v>
+        <v>939</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>906</v>
+        <v>263</v>
       </c>
       <c r="D223" s="13" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
       <c r="E223" s="13" t="s">
-        <v>732</v>
+        <v>742</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
@@ -6996,31 +7005,31 @@
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" s="13" t="s">
-        <v>235</v>
+        <v>936</v>
       </c>
       <c r="C225" s="13" t="s">
-        <v>235</v>
+        <v>912</v>
       </c>
       <c r="D225" s="13" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
       <c r="E225" s="13" t="s">
-        <v>734</v>
+        <v>743</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="B226" s="13" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C226" s="13" t="s">
-        <v>236</v>
+        <v>906</v>
       </c>
       <c r="D226" s="13" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E226" s="13" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
@@ -7041,412 +7050,412 @@
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1"/>
       <c r="B228" s="13" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C228" s="13" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="D228" s="13" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="E228" s="13" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="B229" s="13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C229" s="13" t="s">
-        <v>910</v>
+        <v>235</v>
       </c>
       <c r="D229" s="13" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E229" s="13" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="B230" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C230" s="13" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D230" s="13" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E230" s="13" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="B231" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C231" s="13" t="s">
-        <v>943</v>
+        <v>910</v>
       </c>
       <c r="D231" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E231" s="13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="B232" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>242</v>
+        <v>911</v>
       </c>
       <c r="D232" s="13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E232" s="13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" s="13" t="s">
-        <v>939</v>
+        <v>241</v>
       </c>
       <c r="C233" s="13" t="s">
-        <v>263</v>
+        <v>943</v>
       </c>
       <c r="D233" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E233" s="13" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" s="13" t="s">
-        <v>936</v>
+        <v>236</v>
       </c>
       <c r="C234" s="13" t="s">
-        <v>912</v>
+        <v>236</v>
       </c>
       <c r="D234" s="13" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="E234" s="13" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="B235" s="13" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C235" s="13" t="s">
-        <v>913</v>
+        <v>230</v>
       </c>
       <c r="D235" s="13" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="E235" s="13" t="s">
-        <v>744</v>
+        <v>729</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="B236" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D236" s="13" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E236" s="13" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="B237" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C237" s="13" t="s">
-        <v>245</v>
+        <v>913</v>
       </c>
       <c r="D237" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E237" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1"/>
       <c r="B238" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>914</v>
+        <v>244</v>
       </c>
       <c r="D238" s="13" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E238" s="13" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="B239" s="13" t="s">
-        <v>247</v>
+        <v>34</v>
       </c>
       <c r="C239" s="13" t="s">
-        <v>915</v>
+        <v>34</v>
       </c>
       <c r="D239" s="13" t="s">
-        <v>499</v>
+        <v>273</v>
       </c>
       <c r="E239" s="13" t="s">
-        <v>748</v>
+        <v>522</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="B240" s="13" t="s">
-        <v>248</v>
+        <v>102</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>916</v>
+        <v>813</v>
       </c>
       <c r="D240" s="13" t="s">
-        <v>500</v>
+        <v>344</v>
       </c>
       <c r="E240" s="13" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" s="13" t="s">
-        <v>928</v>
+        <v>247</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>928</v>
+        <v>915</v>
       </c>
       <c r="D241" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E241" s="13" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="B242" s="13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D242" s="13" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E242" s="13" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" s="13" t="s">
-        <v>937</v>
+        <v>944</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="D243" s="13" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E243" s="13" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" s="13" t="s">
-        <v>918</v>
+        <v>246</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="D244" s="13" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E244" s="13" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" s="13" t="s">
-        <v>944</v>
+        <v>248</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="D245" s="13" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E245" s="13" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="B246" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="D246" s="13" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E246" s="13" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="B247" s="13" t="s">
-        <v>251</v>
+        <v>928</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>921</v>
+        <v>928</v>
       </c>
       <c r="D247" s="13" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="E247" s="13" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="B248" s="13" t="s">
-        <v>252</v>
+        <v>937</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>252</v>
+        <v>917</v>
       </c>
       <c r="D248" s="13" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="E248" s="13" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="B249" s="13" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C249" s="13" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D249" s="13" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E249" s="13" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="B250" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C250" s="13" t="s">
-        <v>923</v>
+        <v>252</v>
       </c>
       <c r="D250" s="13" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E250" s="13" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="B251" s="13" t="s">
-        <v>255</v>
+        <v>92</v>
       </c>
       <c r="C251" s="13" t="s">
-        <v>924</v>
+        <v>92</v>
       </c>
       <c r="D251" s="13" t="s">
-        <v>511</v>
+        <v>333</v>
       </c>
       <c r="E251" s="13" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="B252" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C252" s="13" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D252" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E252" s="13" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="B253" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C253" s="13" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D253" s="13" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E253" s="13" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="B254" s="13" t="s">
-        <v>940</v>
+        <v>257</v>
       </c>
       <c r="C254" s="13" t="s">
-        <v>940</v>
+        <v>926</v>
       </c>
       <c r="D254" s="13" t="s">
-        <v>941</v>
+        <v>513</v>
       </c>
       <c r="E254" s="13" t="s">
-        <v>945</v>
-      </c>
-      <c r="F254" t="s">
-        <v>946</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F254">
+    <sortCondition ref="B5:B254"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>